<commit_message>
Actualización cuaderno de estudio con escaleta
Tema 2 grado 8
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,12 +18,118 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="152511" iterateCount="2" iterateDelta="10"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Edgar Josué Malagón Montaña</author>
+  </authors>
+  <commentList>
+    <comment ref="U9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Edgar Josué Malagón Montaña:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Revisar esta parte, este recurso no es aprovechado.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Edgar Josué Malagón Montaña:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Revisar este recurso no es aprovechado, el autor lo construyo.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Edgar Josué Malagón Montaña:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Esto no se habia planteado por el autor, revisar que se utilice de forma adecuada.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Edgar Josué Malagón Montaña:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Revisar esta parte porque este recurso no es aprovechado, el autor lo construyo.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="337">
   <si>
     <t>Asignatura</t>
   </si>
@@ -558,9 +664,6 @@
   </si>
   <si>
     <t>Actividad para reforzar y recordar todo lo aprendido sobre las expresiones algebraicas</t>
-  </si>
-  <si>
-    <t>Es una actividad de carácter propositivo en la que el estudiante debe proponer ejemplos de los tipos de expresiones algebraicas vistas. Se puede complementar el recurso aprovechado</t>
   </si>
   <si>
     <t>Refuerza tu aprendizaje: Las expresiones algebraicas</t>
@@ -697,9 +800,6 @@
     <t>Interactivo que permite estudiar la división sintética y el teorema del residuo</t>
   </si>
   <si>
-    <t>Este interactivo permitirá que el estudiante descubra por qué es válido el teorema del residuo.</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: El teorema del resto</t>
   </si>
   <si>
@@ -715,9 +815,6 @@
     <t>Actividad para reforzar lo visto de la multiplicación y división  de polinomios</t>
   </si>
   <si>
-    <t>Actividad en la que se propone reforzar teórica y prácticamente los conceptos y algoritmos vistos sobre multiplicación y división de polinomios.</t>
-  </si>
-  <si>
     <t>Recurso M101-03</t>
   </si>
   <si>
@@ -1046,13 +1143,25 @@
   </si>
   <si>
     <t>MT_10_06_09</t>
+  </si>
+  <si>
+    <t>Corresponde al REC60 del manuscrito original.</t>
+  </si>
+  <si>
+    <t>Corresponde al REC70 del manuscrito original: Es una actividad de carácter propositivo en la que el estudiante debe proponer ejemplos de los tipos de expresiones algebraicas vistas. Se puede complementar el recurso aprovechado</t>
+  </si>
+  <si>
+    <t>Corresponde al REC170: Actividad en la que se propone reforzar teórica y prácticamente los conceptos y algoritmos vistos sobre multiplicación y división de polinomios.</t>
+  </si>
+  <si>
+    <t>Este interactivo permitirá que el estudiante descubra por qué es válido el teorema del residuo. Se pueden utilizar los ejercicios que planteo el autor en el REC150</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1115,8 +1224,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1217,6 +1339,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1425,15 +1553,6 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1573,6 +1692,18 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1618,17 +1749,14 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1933,12 +2061,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W4" sqref="W4"/>
+      <selection pane="bottomLeft" activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,15 +2077,15 @@
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="30.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="48.42578125" style="101" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="101" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" style="98" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="98" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
     <col min="10" max="10" width="77.7109375" customWidth="1"/>
     <col min="11" max="11" width="18.85546875" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="43" style="107" customWidth="1"/>
+    <col min="15" max="15" width="43" style="104" customWidth="1"/>
     <col min="16" max="16" width="21.5703125" customWidth="1"/>
     <col min="17" max="17" width="16.140625" customWidth="1"/>
     <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -1967,94 +2095,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="6" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="120" t="s">
+      <c r="C1" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="114" t="s">
+      <c r="D1" s="115" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="113" t="s">
+      <c r="E1" s="114" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="121" t="s">
+      <c r="F1" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="115" t="s">
+      <c r="G1" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="110" t="s">
+      <c r="H1" s="111" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="108" t="s">
+      <c r="I1" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="117" t="s">
+      <c r="J1" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="116" t="s">
+      <c r="K1" s="117" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="115" t="s">
+      <c r="L1" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="118" t="s">
+      <c r="M1" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="119"/>
-      <c r="O1" s="112" t="s">
+      <c r="N1" s="120"/>
+      <c r="O1" s="113" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="123" t="s">
+      <c r="P1" s="105" t="s">
         <v>119</v>
       </c>
-      <c r="Q1" s="123" t="s">
+      <c r="Q1" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="126" t="s">
+      <c r="R1" s="108" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="124" t="s">
+      <c r="S1" s="106" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="125" t="s">
+      <c r="T1" s="107" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="124" t="s">
+      <c r="U1" s="106" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="114"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="115"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="116"/>
       <c r="M2" s="7" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="112"/>
-      <c r="P2" s="123"/>
-      <c r="Q2" s="123"/>
-      <c r="R2" s="126"/>
-      <c r="S2" s="124"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="124"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="108"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="107"/>
+      <c r="U2" s="106"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -2095,7 +2223,7 @@
         <v>129</v>
       </c>
       <c r="N3" s="20"/>
-      <c r="O3" s="102" t="s">
+      <c r="O3" s="99" t="s">
         <v>130</v>
       </c>
       <c r="P3" s="19" t="s">
@@ -2156,7 +2284,7 @@
       <c r="N4" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="O4" s="102" t="s">
+      <c r="O4" s="99" t="s">
         <v>141</v>
       </c>
       <c r="P4" s="19" t="s">
@@ -2217,7 +2345,7 @@
       <c r="N5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O5" s="102" t="s">
+      <c r="O5" s="99" t="s">
         <v>149</v>
       </c>
       <c r="P5" s="19" t="s">
@@ -2278,7 +2406,7 @@
       <c r="N6" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="O6" s="103" t="s">
+      <c r="O6" s="100" t="s">
         <v>155</v>
       </c>
       <c r="P6" s="19" t="s">
@@ -2339,7 +2467,7 @@
       <c r="N7" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="O7" s="103" t="s">
+      <c r="O7" s="100" t="s">
         <v>162</v>
       </c>
       <c r="P7" s="19" t="s">
@@ -2400,7 +2528,7 @@
       <c r="N8" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="O8" s="103" t="s">
+      <c r="O8" s="100" t="s">
         <v>166</v>
       </c>
       <c r="P8" s="19" t="s">
@@ -2452,30 +2580,32 @@
         <v>169</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="L9" s="18" t="s">
         <v>140</v>
       </c>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
-      <c r="O9" s="103"/>
-      <c r="P9" s="19" t="s">
+      <c r="O9" s="125" t="s">
+        <v>333</v>
+      </c>
+      <c r="P9" s="124" t="s">
         <v>124</v>
       </c>
-      <c r="Q9" s="32" t="s">
+      <c r="Q9" s="126" t="s">
         <v>171</v>
       </c>
-      <c r="R9" s="33" t="s">
+      <c r="R9" s="126" t="s">
         <v>157</v>
       </c>
-      <c r="S9" s="34" t="s">
+      <c r="S9" s="126" t="s">
         <v>172</v>
       </c>
-      <c r="T9" s="33" t="s">
+      <c r="T9" s="126" t="s">
         <v>173</v>
       </c>
-      <c r="U9" s="34" t="s">
+      <c r="U9" s="126" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2492,7 +2622,7 @@
       <c r="D10" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="32" t="s">
         <v>175</v>
       </c>
       <c r="F10" s="4"/>
@@ -2509,7 +2639,7 @@
         <v>177</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="L10" s="18" t="s">
         <v>140</v>
@@ -2518,25 +2648,25 @@
       <c r="N10" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="103" t="s">
-        <v>178</v>
+      <c r="O10" s="100" t="s">
+        <v>334</v>
       </c>
       <c r="P10" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="Q10" s="32" t="s">
+      <c r="Q10" s="126" t="s">
         <v>171</v>
       </c>
-      <c r="R10" s="33" t="s">
+      <c r="R10" s="126" t="s">
         <v>157</v>
       </c>
-      <c r="S10" s="34" t="s">
+      <c r="S10" s="126" t="s">
         <v>172</v>
       </c>
-      <c r="T10" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="U10" s="34" t="s">
+      <c r="T10" s="126" t="s">
+        <v>178</v>
+      </c>
+      <c r="U10" s="126" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2551,14 +2681,14 @@
         <v>122</v>
       </c>
       <c r="D11" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="32" t="s">
         <v>180</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>181</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H11" s="14">
         <v>9</v>
@@ -2567,7 +2697,7 @@
         <v>131</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>127</v>
@@ -2579,8 +2709,8 @@
       <c r="N11" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="O11" s="103" t="s">
-        <v>184</v>
+      <c r="O11" s="100" t="s">
+        <v>183</v>
       </c>
       <c r="P11" s="19" t="s">
         <v>124</v>
@@ -2595,7 +2725,7 @@
         <v>143</v>
       </c>
       <c r="T11" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U11" s="24" t="s">
         <v>145</v>
@@ -2612,14 +2742,14 @@
         <v>122</v>
       </c>
       <c r="D12" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="E12" s="32" t="s">
         <v>180</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>181</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H12" s="14">
         <v>10</v>
@@ -2628,7 +2758,7 @@
         <v>124</v>
       </c>
       <c r="J12" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K12" s="14" t="s">
         <v>154</v>
@@ -2637,29 +2767,29 @@
         <v>128</v>
       </c>
       <c r="M12" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="N12" s="19"/>
+      <c r="O12" s="100" t="s">
         <v>188</v>
-      </c>
-      <c r="N12" s="19"/>
-      <c r="O12" s="103" t="s">
-        <v>189</v>
       </c>
       <c r="P12" s="19" t="s">
         <v>131</v>
       </c>
       <c r="Q12" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="R12" s="23" t="s">
         <v>157</v>
       </c>
       <c r="S12" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="T12" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="T12" s="25" t="s">
+      <c r="U12" s="24" t="s">
         <v>192</v>
-      </c>
-      <c r="U12" s="24" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -2673,14 +2803,14 @@
         <v>122</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="E13" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="E13" s="32" t="s">
         <v>175</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H13" s="14">
         <v>11</v>
@@ -2689,7 +2819,7 @@
         <v>131</v>
       </c>
       <c r="J13" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K13" s="14" t="s">
         <v>127</v>
@@ -2701,8 +2831,8 @@
       <c r="N13" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="O13" s="103" t="s">
-        <v>196</v>
+      <c r="O13" s="100" t="s">
+        <v>195</v>
       </c>
       <c r="P13" s="19" t="s">
         <v>124</v>
@@ -2717,7 +2847,7 @@
         <v>143</v>
       </c>
       <c r="T13" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="U13" s="24" t="s">
         <v>145</v>
@@ -2734,14 +2864,14 @@
         <v>122</v>
       </c>
       <c r="D14" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="32" t="s">
         <v>198</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>199</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H14" s="14">
         <v>12</v>
@@ -2750,7 +2880,7 @@
         <v>131</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>127</v>
@@ -2762,8 +2892,8 @@
       <c r="N14" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="O14" s="103" t="s">
-        <v>202</v>
+      <c r="O14" s="100" t="s">
+        <v>201</v>
       </c>
       <c r="P14" s="19" t="s">
         <v>124</v>
@@ -2778,7 +2908,7 @@
         <v>143</v>
       </c>
       <c r="T14" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U14" s="24" t="s">
         <v>145</v>
@@ -2795,14 +2925,14 @@
         <v>122</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>204</v>
+        <v>197</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>203</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H15" s="14">
         <v>13</v>
@@ -2811,7 +2941,7 @@
         <v>131</v>
       </c>
       <c r="J15" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K15" s="14" t="s">
         <v>127</v>
@@ -2823,8 +2953,8 @@
       <c r="N15" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="O15" s="103" t="s">
-        <v>207</v>
+      <c r="O15" s="100" t="s">
+        <v>206</v>
       </c>
       <c r="P15" s="19" t="s">
         <v>124</v>
@@ -2839,7 +2969,7 @@
         <v>143</v>
       </c>
       <c r="T15" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U15" s="24" t="s">
         <v>145</v>
@@ -2856,14 +2986,14 @@
         <v>122</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>209</v>
+        <v>197</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>208</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H16" s="14">
         <v>14</v>
@@ -2872,7 +3002,7 @@
         <v>124</v>
       </c>
       <c r="J16" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K16" s="14" t="s">
         <v>127</v>
@@ -2881,11 +3011,11 @@
         <v>128</v>
       </c>
       <c r="M16" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="N16" s="19"/>
+      <c r="O16" s="100" t="s">
         <v>211</v>
-      </c>
-      <c r="N16" s="19"/>
-      <c r="O16" s="103" t="s">
-        <v>212</v>
       </c>
       <c r="P16" s="19" t="s">
         <v>131</v>
@@ -2900,7 +3030,7 @@
         <v>133</v>
       </c>
       <c r="T16" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U16" s="24" t="s">
         <v>135</v>
@@ -2917,14 +3047,14 @@
         <v>122</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>209</v>
+        <v>197</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>208</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H17" s="14">
         <v>15</v>
@@ -2933,7 +3063,7 @@
         <v>131</v>
       </c>
       <c r="J17" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K17" s="14" t="s">
         <v>154</v>
@@ -2945,8 +3075,8 @@
       <c r="N17" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="O17" s="103" t="s">
-        <v>216</v>
+      <c r="O17" s="100" t="s">
+        <v>215</v>
       </c>
       <c r="P17" s="19" t="s">
         <v>124</v>
@@ -2961,7 +3091,7 @@
         <v>158</v>
       </c>
       <c r="T17" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="U17" s="24" t="s">
         <v>159</v>
@@ -2978,14 +3108,14 @@
         <v>122</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>209</v>
+        <v>197</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>208</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H18" s="14">
         <v>16</v>
@@ -2993,19 +3123,19 @@
       <c r="I18" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="J18" s="36" t="s">
-        <v>218</v>
-      </c>
-      <c r="K18" s="37" t="s">
+      <c r="J18" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="K18" s="34" t="s">
         <v>154</v>
       </c>
       <c r="L18" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="M18" s="38"/>
+      <c r="M18" s="35"/>
       <c r="N18" s="19"/>
-      <c r="O18" s="103" t="s">
-        <v>219</v>
+      <c r="O18" s="100" t="s">
+        <v>336</v>
       </c>
       <c r="P18" s="19" t="s">
         <v>124</v>
@@ -3020,7 +3150,7 @@
         <v>158</v>
       </c>
       <c r="T18" s="25" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="U18" s="24" t="s">
         <v>159</v>
@@ -3037,14 +3167,14 @@
         <v>122</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>209</v>
+        <v>197</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>208</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="28" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H19" s="14">
         <v>17</v>
@@ -3053,10 +3183,10 @@
         <v>131</v>
       </c>
       <c r="J19" s="29" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="L19" s="18" t="s">
         <v>140</v>
@@ -3065,25 +3195,25 @@
       <c r="N19" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="O19" s="103" t="s">
-        <v>222</v>
+      <c r="O19" s="100" t="s">
+        <v>220</v>
       </c>
       <c r="P19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="Q19" s="22" t="s">
+      <c r="Q19" s="124" t="s">
         <v>156</v>
       </c>
-      <c r="R19" s="23" t="s">
+      <c r="R19" s="124" t="s">
         <v>157</v>
       </c>
-      <c r="S19" s="24" t="s">
+      <c r="S19" s="124" t="s">
         <v>158</v>
       </c>
-      <c r="T19" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="U19" s="24" t="s">
+      <c r="T19" s="124" t="s">
+        <v>219</v>
+      </c>
+      <c r="U19" s="124" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3098,14 +3228,14 @@
         <v>122</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="E20" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="E20" s="32" t="s">
         <v>175</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="28" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H20" s="14">
         <v>18</v>
@@ -3114,7 +3244,7 @@
         <v>131</v>
       </c>
       <c r="J20" s="29" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K20" s="14" t="s">
         <v>127</v>
@@ -3126,8 +3256,8 @@
       <c r="N20" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="O20" s="103" t="s">
-        <v>225</v>
+      <c r="O20" s="100" t="s">
+        <v>335</v>
       </c>
       <c r="P20" s="19" t="s">
         <v>131</v>
@@ -3142,7 +3272,7 @@
         <v>143</v>
       </c>
       <c r="T20" s="25" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="U20" s="24" t="s">
         <v>145</v>
@@ -3159,14 +3289,14 @@
         <v>122</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="E21" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="E21" s="32" t="s">
         <v>175</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="28" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H21" s="14">
         <v>19</v>
@@ -3175,7 +3305,7 @@
         <v>131</v>
       </c>
       <c r="J21" s="29" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="K21" s="14" t="s">
         <v>127</v>
@@ -3187,8 +3317,8 @@
       <c r="N21" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="O21" s="103" t="s">
-        <v>230</v>
+      <c r="O21" s="100" t="s">
+        <v>227</v>
       </c>
       <c r="P21" s="19" t="s">
         <v>131</v>
@@ -3203,7 +3333,7 @@
         <v>143</v>
       </c>
       <c r="T21" s="25" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="U21" s="24" t="s">
         <v>145</v>
@@ -3220,14 +3350,14 @@
         <v>122</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="E22" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="E22" s="32" t="s">
         <v>175</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="28" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H22" s="14">
         <v>20</v>
@@ -3235,8 +3365,8 @@
       <c r="I22" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J22" s="36" t="s">
-        <v>234</v>
+      <c r="J22" s="33" t="s">
+        <v>231</v>
       </c>
       <c r="K22" s="14" t="s">
         <v>127</v>
@@ -3248,8 +3378,8 @@
       <c r="N22" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="O22" s="103" t="s">
-        <v>235</v>
+      <c r="O22" s="100" t="s">
+        <v>232</v>
       </c>
       <c r="P22" s="19" t="s">
         <v>124</v>
@@ -3264,14 +3394,14 @@
         <v>143</v>
       </c>
       <c r="T22" s="25" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="U22" s="24" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="36" t="s">
         <v>120</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -3280,15 +3410,15 @@
       <c r="C23" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>238</v>
+      <c r="D23" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>235</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="18" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H23" s="14">
         <v>21</v>
@@ -3297,20 +3427,20 @@
         <v>131</v>
       </c>
       <c r="J23" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="K23" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="K23" s="39" t="s">
         <v>127</v>
       </c>
       <c r="L23" s="15" t="s">
         <v>128</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="N23" s="20"/>
-      <c r="O23" s="103" t="s">
-        <v>242</v>
+      <c r="O23" s="100" t="s">
+        <v>239</v>
       </c>
       <c r="P23" s="19" t="s">
         <v>131</v>
@@ -3325,14 +3455,14 @@
         <v>133</v>
       </c>
       <c r="T23" s="25" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="U23" s="24" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="36" t="s">
         <v>120</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -3341,15 +3471,15 @@
       <c r="C24" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="40" t="s">
-        <v>244</v>
-      </c>
-      <c r="E24" s="35" t="s">
-        <v>238</v>
+      <c r="D24" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>235</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H24" s="14">
         <v>22</v>
@@ -3358,9 +3488,9 @@
         <v>131</v>
       </c>
       <c r="J24" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="K24" s="43" t="s">
+        <v>242</v>
+      </c>
+      <c r="K24" s="40" t="s">
         <v>154</v>
       </c>
       <c r="L24" s="15" t="s">
@@ -3370,30 +3500,30 @@
       <c r="N24" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="O24" s="103" t="s">
-        <v>246</v>
+      <c r="O24" s="100" t="s">
+        <v>243</v>
       </c>
       <c r="P24" s="19" t="s">
         <v>124</v>
       </c>
       <c r="Q24" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="R24" s="23" t="s">
         <v>157</v>
       </c>
       <c r="S24" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="T24" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="T24" s="25" t="s">
+      <c r="U24" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="U24" s="24" t="s">
-        <v>193</v>
-      </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="36" t="s">
         <v>120</v>
       </c>
       <c r="B25" s="9" t="s">
@@ -3402,15 +3532,15 @@
       <c r="C25" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="40" t="s">
-        <v>244</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>238</v>
+      <c r="D25" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>235</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="18" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H25" s="14">
         <v>23</v>
@@ -3419,9 +3549,9 @@
         <v>131</v>
       </c>
       <c r="J25" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="K25" s="42" t="s">
+        <v>245</v>
+      </c>
+      <c r="K25" s="39" t="s">
         <v>127</v>
       </c>
       <c r="L25" s="15" t="s">
@@ -3431,8 +3561,8 @@
       <c r="N25" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="O25" s="103" t="s">
-        <v>249</v>
+      <c r="O25" s="100" t="s">
+        <v>246</v>
       </c>
       <c r="P25" s="19" t="s">
         <v>124</v>
@@ -3447,14 +3577,14 @@
         <v>143</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="U25" s="24" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="36" t="s">
         <v>120</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -3463,10 +3593,10 @@
       <c r="C26" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="40" t="s">
-        <v>244</v>
-      </c>
-      <c r="E26" s="35" t="s">
+      <c r="D26" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="E26" s="32" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="4"/>
@@ -3479,29 +3609,29 @@
       <c r="I26" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J26" s="44" t="s">
-        <v>251</v>
-      </c>
-      <c r="K26" s="42" t="s">
+      <c r="J26" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="K26" s="39" t="s">
         <v>127</v>
       </c>
       <c r="L26" s="15" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
-      <c r="O26" s="103" t="s">
-        <v>253</v>
-      </c>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="47"/>
-      <c r="S26" s="48"/>
-      <c r="T26" s="49"/>
-      <c r="U26" s="48"/>
+      <c r="O26" s="100" t="s">
+        <v>250</v>
+      </c>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="45"/>
+      <c r="T26" s="46"/>
+      <c r="U26" s="45"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="36" t="s">
         <v>120</v>
       </c>
       <c r="B27" s="9" t="s">
@@ -3510,15 +3640,15 @@
       <c r="C27" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="E27" s="35" t="s">
-        <v>254</v>
+      <c r="D27" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>251</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="18" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H27" s="14">
         <v>25</v>
@@ -3527,20 +3657,20 @@
         <v>131</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="K27" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="K27" s="39" t="s">
         <v>127</v>
       </c>
       <c r="L27" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="M27" s="51"/>
+      <c r="M27" s="48"/>
       <c r="N27" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O27" s="102" t="s">
-        <v>258</v>
+      <c r="O27" s="99" t="s">
+        <v>255</v>
       </c>
       <c r="P27" s="19" t="s">
         <v>124</v>
@@ -3555,14 +3685,14 @@
         <v>133</v>
       </c>
       <c r="T27" s="25" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="U27" s="24" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="36" t="s">
         <v>120</v>
       </c>
       <c r="B28" s="9" t="s">
@@ -3571,11 +3701,11 @@
       <c r="C28" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="E28" s="35" t="s">
-        <v>260</v>
+      <c r="D28" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>257</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="18"/>
@@ -3584,203 +3714,203 @@
       </c>
       <c r="I28" s="17"/>
       <c r="J28" s="16"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="102"/>
-      <c r="P28" s="53"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="99"/>
+      <c r="P28" s="50"/>
       <c r="Q28" s="21"/>
-      <c r="R28" s="54"/>
-      <c r="S28" s="55"/>
-      <c r="T28" s="56"/>
-      <c r="U28" s="55"/>
+      <c r="R28" s="51"/>
+      <c r="S28" s="52"/>
+      <c r="T28" s="53"/>
+      <c r="U28" s="52"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="57"/>
-      <c r="B29" s="58"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="58"/>
+      <c r="A29" s="54"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="55"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="63"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="66"/>
-      <c r="L29" s="65"/>
-      <c r="M29" s="67"/>
-      <c r="N29" s="67"/>
-      <c r="O29" s="104"/>
-      <c r="P29" s="69"/>
-      <c r="Q29" s="68"/>
-      <c r="R29" s="70"/>
-      <c r="S29" s="71"/>
-      <c r="T29" s="72"/>
-      <c r="U29" s="71"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="101"/>
+      <c r="P29" s="66"/>
+      <c r="Q29" s="65"/>
+      <c r="R29" s="67"/>
+      <c r="S29" s="68"/>
+      <c r="T29" s="69"/>
+      <c r="U29" s="68"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="57"/>
-      <c r="B30" s="73"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="73"/>
+      <c r="A30" s="54"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="70"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="78"/>
-      <c r="J30" s="79"/>
-      <c r="K30" s="66"/>
-      <c r="L30" s="65"/>
-      <c r="M30" s="67"/>
-      <c r="N30" s="67"/>
-      <c r="O30" s="105"/>
-      <c r="P30" s="81"/>
-      <c r="Q30" s="80"/>
-      <c r="R30" s="82"/>
-      <c r="S30" s="83"/>
-      <c r="T30" s="84"/>
-      <c r="U30" s="83"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="62"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="102"/>
+      <c r="P30" s="78"/>
+      <c r="Q30" s="77"/>
+      <c r="R30" s="79"/>
+      <c r="S30" s="80"/>
+      <c r="T30" s="81"/>
+      <c r="U30" s="80"/>
     </row>
     <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="85"/>
-      <c r="B31" s="86"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="86"/>
+      <c r="A31" s="82"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="84"/>
+      <c r="D31" s="85"/>
+      <c r="E31" s="83"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="89"/>
-      <c r="H31" s="90"/>
-      <c r="I31" s="91"/>
-      <c r="J31" s="92"/>
-      <c r="K31" s="94"/>
-      <c r="L31" s="93"/>
-      <c r="M31" s="95"/>
-      <c r="N31" s="95"/>
-      <c r="O31" s="106"/>
-      <c r="P31" s="97"/>
-      <c r="Q31" s="96"/>
-      <c r="R31" s="98"/>
-      <c r="S31" s="99"/>
-      <c r="T31" s="100"/>
-      <c r="U31" s="99"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="87"/>
+      <c r="I31" s="88"/>
+      <c r="J31" s="89"/>
+      <c r="K31" s="91"/>
+      <c r="L31" s="90"/>
+      <c r="M31" s="92"/>
+      <c r="N31" s="92"/>
+      <c r="O31" s="103"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="93"/>
+      <c r="R31" s="95"/>
+      <c r="S31" s="96"/>
+      <c r="T31" s="97"/>
+      <c r="U31" s="96"/>
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="85"/>
-      <c r="B32" s="86"/>
-      <c r="C32" s="87"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="86"/>
+      <c r="A32" s="82"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="85"/>
+      <c r="E32" s="83"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="89"/>
-      <c r="H32" s="90"/>
-      <c r="I32" s="91"/>
-      <c r="J32" s="92"/>
-      <c r="K32" s="94"/>
-      <c r="L32" s="93"/>
-      <c r="M32" s="95"/>
-      <c r="N32" s="95"/>
-      <c r="O32" s="106"/>
-      <c r="P32" s="97"/>
-      <c r="Q32" s="96"/>
-      <c r="R32" s="98"/>
-      <c r="S32" s="99"/>
-      <c r="T32" s="100"/>
-      <c r="U32" s="99"/>
+      <c r="G32" s="86"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="88"/>
+      <c r="J32" s="89"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="90"/>
+      <c r="M32" s="92"/>
+      <c r="N32" s="92"/>
+      <c r="O32" s="103"/>
+      <c r="P32" s="94"/>
+      <c r="Q32" s="93"/>
+      <c r="R32" s="95"/>
+      <c r="S32" s="96"/>
+      <c r="T32" s="97"/>
+      <c r="U32" s="96"/>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="85"/>
-      <c r="B33" s="86"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="86"/>
+      <c r="A33" s="82"/>
+      <c r="B33" s="83"/>
+      <c r="C33" s="84"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="83"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="89"/>
-      <c r="H33" s="90"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="92"/>
-      <c r="K33" s="94"/>
-      <c r="L33" s="93"/>
-      <c r="M33" s="95"/>
-      <c r="N33" s="95"/>
-      <c r="O33" s="106"/>
-      <c r="P33" s="97"/>
-      <c r="Q33" s="96"/>
-      <c r="R33" s="98"/>
-      <c r="S33" s="99"/>
-      <c r="T33" s="100"/>
-      <c r="U33" s="99"/>
+      <c r="G33" s="86"/>
+      <c r="H33" s="87"/>
+      <c r="I33" s="88"/>
+      <c r="J33" s="89"/>
+      <c r="K33" s="91"/>
+      <c r="L33" s="90"/>
+      <c r="M33" s="92"/>
+      <c r="N33" s="92"/>
+      <c r="O33" s="103"/>
+      <c r="P33" s="94"/>
+      <c r="Q33" s="93"/>
+      <c r="R33" s="95"/>
+      <c r="S33" s="96"/>
+      <c r="T33" s="97"/>
+      <c r="U33" s="96"/>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="85"/>
-      <c r="B34" s="86"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="86"/>
+      <c r="A34" s="82"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="84"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="83"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="89"/>
-      <c r="H34" s="90"/>
-      <c r="I34" s="91"/>
-      <c r="J34" s="92"/>
-      <c r="K34" s="94"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="95"/>
-      <c r="N34" s="95"/>
-      <c r="O34" s="106"/>
-      <c r="P34" s="97"/>
-      <c r="Q34" s="96"/>
-      <c r="R34" s="98"/>
-      <c r="S34" s="99"/>
-      <c r="T34" s="100"/>
-      <c r="U34" s="99"/>
+      <c r="G34" s="86"/>
+      <c r="H34" s="87"/>
+      <c r="I34" s="88"/>
+      <c r="J34" s="89"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="90"/>
+      <c r="M34" s="92"/>
+      <c r="N34" s="92"/>
+      <c r="O34" s="103"/>
+      <c r="P34" s="94"/>
+      <c r="Q34" s="93"/>
+      <c r="R34" s="95"/>
+      <c r="S34" s="96"/>
+      <c r="T34" s="97"/>
+      <c r="U34" s="96"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="85"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="87"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="86"/>
+      <c r="A35" s="82"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="83"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="90"/>
-      <c r="I35" s="91"/>
-      <c r="J35" s="92"/>
-      <c r="K35" s="94"/>
-      <c r="L35" s="93"/>
-      <c r="M35" s="95"/>
-      <c r="N35" s="95"/>
-      <c r="O35" s="106"/>
-      <c r="P35" s="97"/>
-      <c r="Q35" s="96"/>
-      <c r="R35" s="98"/>
-      <c r="S35" s="99"/>
-      <c r="T35" s="100"/>
-      <c r="U35" s="99"/>
+      <c r="G35" s="86"/>
+      <c r="H35" s="87"/>
+      <c r="I35" s="88"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="91"/>
+      <c r="L35" s="90"/>
+      <c r="M35" s="92"/>
+      <c r="N35" s="92"/>
+      <c r="O35" s="103"/>
+      <c r="P35" s="94"/>
+      <c r="Q35" s="93"/>
+      <c r="R35" s="95"/>
+      <c r="S35" s="96"/>
+      <c r="T35" s="97"/>
+      <c r="U35" s="96"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C37" t="s">
         <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E37" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F37" s="4"/>
-      <c r="G37" s="101" t="s">
-        <v>264</v>
+      <c r="G37" s="98" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C38" t="s">
         <v>127</v>
@@ -3792,49 +3922,49 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>263</v>
+      </c>
+      <c r="C39" t="s">
+        <v>264</v>
+      </c>
+      <c r="D39" t="s">
+        <v>265</v>
+      </c>
+      <c r="E39" t="s">
         <v>266</v>
       </c>
-      <c r="C39" t="s">
-        <v>267</v>
-      </c>
-      <c r="D39" t="s">
-        <v>268</v>
-      </c>
-      <c r="E39" t="s">
-        <v>269</v>
-      </c>
       <c r="F39" s="4"/>
-      <c r="G39" s="101" t="s">
+      <c r="G39" s="98" t="s">
         <v>128</v>
       </c>
       <c r="J39" t="s">
         <v>140</v>
       </c>
       <c r="K39" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E43" t="s">
         <v>126</v>
@@ -3843,16 +3973,16 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E44" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E45" t="s">
         <v>148</v>
@@ -3861,7 +3991,7 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E46" t="s">
         <v>170</v>
@@ -3879,37 +4009,37 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F53" s="4"/>
     </row>
@@ -3918,7 +4048,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F55" s="4"/>
     </row>
@@ -4166,277 +4296,277 @@
     </row>
     <row r="113" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4561,12 +4691,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4581,6 +4705,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L35">
@@ -4601,6 +4731,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Formulas nuevas de mat 8 guion 1
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -52,31 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Edgar Josué Malagón Montaña:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Revisar este recurso no es aprovechado, el autor lo construyo.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U18" authorId="0" shapeId="0">
+    <comment ref="U20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q19" authorId="0" shapeId="0">
+    <comment ref="Q21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="344">
   <si>
     <t>Asignatura</t>
   </si>
@@ -660,9 +636,6 @@
     <t>Consolidación</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: las expresiones algebraicas</t>
-  </si>
-  <si>
     <t>Actividad para reforzar y recordar todo lo aprendido sobre las expresiones algebraicas</t>
   </si>
   <si>
@@ -709,9 +682,6 @@
   </si>
   <si>
     <t>MT_09_02</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: la adición de polinomios</t>
   </si>
   <si>
     <t>Actividad para reforzar lo visto de la adición de polinomios</t>
@@ -809,9 +779,6 @@
     <t>Actividad para resolver problemas usando el teorema del residuo</t>
   </si>
   <si>
-    <t>Refuerza el aprendizaje: la división y la multiplicación de polinomios</t>
-  </si>
-  <si>
     <t>Actividad para reforzar lo visto de la multiplicación y división  de polinomios</t>
   </si>
   <si>
@@ -914,9 +881,6 @@
     <t>Corresponde al REC230 propuesto por el autor. Se propone un test matemático que incluye diversas situaciones problema, con el objeto de seleccionar la respuesta apropiada.</t>
   </si>
   <si>
-    <t>Recurso M7A-02</t>
-  </si>
-  <si>
     <t>Webs de referencia</t>
   </si>
   <si>
@@ -1155,13 +1119,46 @@
   </si>
   <si>
     <t>Este interactivo permitirá que el estudiante descubra por qué es válido el teorema del residuo. Se pueden utilizar los ejercicios que planteo el autor en el REC150</t>
+  </si>
+  <si>
+    <t>Recurso M101-01</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las operaciones aditivas entre polinomios</t>
+  </si>
+  <si>
+    <t>Introducción a las expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Resuelve problemas con las operaciones con expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Refuerza el aprendizaje: La multiplicación y la división de polinomuos</t>
+  </si>
+  <si>
+    <t>Actividad para resolver situacionmes aplicando las operacione entre polinomios</t>
+  </si>
+  <si>
+    <t>Recurso M5A-02</t>
+  </si>
+  <si>
+    <t>Ver plataforma España</t>
+  </si>
+  <si>
+    <t>¿Qué sabes de las expresiones algebraicas?</t>
+  </si>
+  <si>
+    <t>Proponer problemas de áreas y dimensiones de cuerpos en donde se requiera aplicar las operaciones de expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Recurso M5A-03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1236,6 +1233,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="19">
@@ -1468,7 +1473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1704,6 +1709,15 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1749,13 +1763,22 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2062,29 +2085,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U284"/>
+  <dimension ref="A1:U286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U9" sqref="U9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="30.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="48.42578125" style="98" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="98" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="77.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="98" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="98" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="77.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="7.85546875" customWidth="1"/>
     <col min="15" max="15" width="43" style="104" customWidth="1"/>
     <col min="16" max="16" width="21.5703125" customWidth="1"/>
     <col min="17" max="17" width="16.140625" customWidth="1"/>
@@ -2095,94 +2117,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="6" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="121" t="s">
+      <c r="C1" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="115" t="s">
+      <c r="D1" s="118" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="114" t="s">
+      <c r="E1" s="117" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="122" t="s">
+      <c r="F1" s="125" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="116" t="s">
+      <c r="G1" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="111" t="s">
+      <c r="H1" s="114" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="109" t="s">
+      <c r="I1" s="112" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="118" t="s">
+      <c r="J1" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="117" t="s">
+      <c r="K1" s="120" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="116" t="s">
+      <c r="L1" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="119" t="s">
+      <c r="M1" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="120"/>
-      <c r="O1" s="113" t="s">
+      <c r="N1" s="123"/>
+      <c r="O1" s="116" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="105" t="s">
+      <c r="P1" s="127" t="s">
         <v>119</v>
       </c>
-      <c r="Q1" s="105" t="s">
+      <c r="Q1" s="127" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="108" t="s">
+      <c r="R1" s="130" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="106" t="s">
+      <c r="S1" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="107" t="s">
+      <c r="T1" s="129" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="106" t="s">
+      <c r="U1" s="128" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="116"/>
+      <c r="A2" s="118"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="119"/>
       <c r="M2" s="7" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="113"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="108"/>
-      <c r="S2" s="106"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="106"/>
+      <c r="O2" s="116"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="130"/>
+      <c r="S2" s="128"/>
+      <c r="T2" s="129"/>
+      <c r="U2" s="128"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -2202,7 +2224,7 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="13" t="s">
-        <v>123</v>
+        <v>335</v>
       </c>
       <c r="H3" s="14">
         <v>1</v>
@@ -2227,7 +2249,7 @@
         <v>130</v>
       </c>
       <c r="P3" s="19" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="Q3" s="22">
         <v>8</v>
@@ -2587,86 +2609,66 @@
       </c>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
-      <c r="O9" s="125" t="s">
-        <v>333</v>
-      </c>
-      <c r="P9" s="124" t="s">
+      <c r="O9" s="111" t="s">
+        <v>329</v>
+      </c>
+      <c r="P9" s="110" t="s">
         <v>124</v>
       </c>
-      <c r="Q9" s="126" t="s">
+      <c r="Q9" s="131" t="s">
         <v>171</v>
       </c>
-      <c r="R9" s="126" t="s">
+      <c r="R9" s="131" t="s">
         <v>157</v>
       </c>
-      <c r="S9" s="126" t="s">
+      <c r="S9" s="131" t="s">
         <v>172</v>
       </c>
-      <c r="T9" s="126" t="s">
+      <c r="T9" s="131" t="s">
         <v>173</v>
       </c>
-      <c r="U9" s="126" t="s">
+      <c r="U9" s="131" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>175</v>
-      </c>
+      <c r="A10" s="26"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="109"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="H10" s="14">
-        <v>8</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>131</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="18"/>
       <c r="J10" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L10" s="18" t="s">
-        <v>140</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="18"/>
       <c r="M10" s="19"/>
-      <c r="N10" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="O10" s="100" t="s">
-        <v>334</v>
-      </c>
-      <c r="P10" s="19" t="s">
+      <c r="N10" s="19"/>
+      <c r="O10" s="111" t="s">
+        <v>340</v>
+      </c>
+      <c r="P10" s="110" t="s">
         <v>124</v>
       </c>
-      <c r="Q10" s="126" t="s">
+      <c r="Q10" s="132" t="s">
         <v>171</v>
       </c>
-      <c r="R10" s="126" t="s">
+      <c r="R10" s="132" t="s">
         <v>157</v>
       </c>
-      <c r="S10" s="126" t="s">
+      <c r="S10" s="132" t="s">
         <v>172</v>
       </c>
-      <c r="T10" s="126" t="s">
-        <v>178</v>
-      </c>
-      <c r="U10" s="126" t="s">
+      <c r="T10" s="132" t="s">
+        <v>341</v>
+      </c>
+      <c r="U10" s="132" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2681,23 +2683,23 @@
         <v>122</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="28" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H11" s="14">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>131</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>127</v>
@@ -2706,28 +2708,28 @@
         <v>140</v>
       </c>
       <c r="M11" s="19"/>
-      <c r="N11" s="19" t="s">
-        <v>95</v>
+      <c r="N11" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="O11" s="100" t="s">
-        <v>183</v>
+        <v>330</v>
       </c>
       <c r="P11" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="Q11" s="105">
         <v>8</v>
       </c>
-      <c r="R11" s="23" t="s">
+      <c r="R11" s="108" t="s">
         <v>142</v>
       </c>
-      <c r="S11" s="24" t="s">
+      <c r="S11" s="106" t="s">
         <v>143</v>
       </c>
-      <c r="T11" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="U11" s="24" t="s">
+      <c r="T11" s="107" t="s">
+        <v>333</v>
+      </c>
+      <c r="U11" s="106" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2742,54 +2744,54 @@
         <v>122</v>
       </c>
       <c r="D12" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="32" t="s">
         <v>179</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>180</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="28" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H12" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I12" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="O12" s="100" t="s">
+        <v>182</v>
+      </c>
+      <c r="P12" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="J12" s="29" t="s">
-        <v>186</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="M12" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="N12" s="19"/>
-      <c r="O12" s="100" t="s">
-        <v>188</v>
-      </c>
-      <c r="P12" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q12" s="22" t="s">
-        <v>189</v>
+      <c r="Q12" s="22">
+        <v>8</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="S12" s="24" t="s">
-        <v>190</v>
+        <v>143</v>
       </c>
       <c r="T12" s="25" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="U12" s="24" t="s">
-        <v>192</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -2803,54 +2805,54 @@
         <v>122</v>
       </c>
       <c r="D13" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="32" t="s">
         <v>179</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>175</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="28" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="H13" s="14">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I13" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="J13" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="N13" s="19"/>
+      <c r="O13" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="P13" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="J13" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="O13" s="100" t="s">
-        <v>195</v>
-      </c>
-      <c r="P13" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q13" s="22">
-        <v>8</v>
+      <c r="Q13" s="22" t="s">
+        <v>188</v>
       </c>
       <c r="R13" s="23" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="S13" s="24" t="s">
-        <v>143</v>
+        <v>189</v>
       </c>
       <c r="T13" s="25" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="U13" s="24" t="s">
-        <v>145</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -2864,23 +2866,23 @@
         <v>122</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="28" t="s">
-        <v>199</v>
+        <v>334</v>
       </c>
       <c r="H14" s="14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I14" s="18" t="s">
         <v>131</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>127</v>
@@ -2890,10 +2892,10 @@
       </c>
       <c r="M14" s="19"/>
       <c r="N14" s="19" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="O14" s="100" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="P14" s="19" t="s">
         <v>124</v>
@@ -2908,14 +2910,14 @@
         <v>143</v>
       </c>
       <c r="T14" s="25" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="U14" s="24" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="26" t="s">
         <v>120</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -2925,23 +2927,23 @@
         <v>122</v>
       </c>
       <c r="D15" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="E15" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="13" t="s">
-        <v>204</v>
-      </c>
       <c r="H15" s="14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>131</v>
       </c>
       <c r="J15" s="29" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="K15" s="14" t="s">
         <v>127</v>
@@ -2950,11 +2952,11 @@
         <v>140</v>
       </c>
       <c r="M15" s="19"/>
-      <c r="N15" s="7" t="s">
-        <v>97</v>
+      <c r="N15" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="O15" s="100" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="P15" s="19" t="s">
         <v>124</v>
@@ -2969,14 +2971,14 @@
         <v>143</v>
       </c>
       <c r="T15" s="25" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="U15" s="24" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="31" t="s">
         <v>120</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -2986,54 +2988,54 @@
         <v>122</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="28" t="s">
-        <v>208</v>
+      <c r="G16" s="13" t="s">
+        <v>202</v>
       </c>
       <c r="H16" s="14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="J16" s="29" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="K16" s="14" t="s">
         <v>127</v>
       </c>
       <c r="L16" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="M16" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="N16" s="19"/>
+        <v>140</v>
+      </c>
+      <c r="M16" s="19"/>
+      <c r="N16" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="O16" s="100" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="Q16" s="22">
         <v>8</v>
       </c>
       <c r="R16" s="23" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="S16" s="24" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="T16" s="25" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="U16" s="24" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -3047,54 +3049,54 @@
         <v>122</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E17" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="H17" s="14">
+        <v>14</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="M17" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="H17" s="14">
-        <v>15</v>
-      </c>
-      <c r="I17" s="18" t="s">
+      <c r="N17" s="19"/>
+      <c r="O17" s="100" t="s">
+        <v>209</v>
+      </c>
+      <c r="P17" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="J17" s="29" t="s">
-        <v>214</v>
-      </c>
-      <c r="K17" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="L17" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="O17" s="100" t="s">
-        <v>215</v>
-      </c>
-      <c r="P17" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q17" s="22" t="s">
-        <v>156</v>
+      <c r="Q17" s="22">
+        <v>8</v>
       </c>
       <c r="R17" s="23" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="S17" s="24" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="T17" s="25" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="U17" s="24" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -3108,34 +3110,36 @@
         <v>122</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="13" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H18" s="14">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="J18" s="33" t="s">
-        <v>217</v>
-      </c>
-      <c r="K18" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="K18" s="14" t="s">
         <v>154</v>
       </c>
       <c r="L18" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="M18" s="35"/>
-      <c r="N18" s="19"/>
+        <v>140</v>
+      </c>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19" t="s">
+        <v>103</v>
+      </c>
       <c r="O18" s="100" t="s">
-        <v>336</v>
+        <v>213</v>
       </c>
       <c r="P18" s="19" t="s">
         <v>124</v>
@@ -3150,71 +3154,53 @@
         <v>158</v>
       </c>
       <c r="T18" s="25" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="U18" s="24" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>208</v>
-      </c>
+      <c r="A19" s="26"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="H19" s="14">
-        <v>17</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>131</v>
-      </c>
+      <c r="G19" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="18"/>
       <c r="J19" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="K19" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L19" s="18" t="s">
-        <v>140</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="K19" s="14"/>
+      <c r="L19" s="18"/>
       <c r="M19" s="19"/>
       <c r="N19" s="19" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="O19" s="100" t="s">
-        <v>220</v>
+        <v>342</v>
       </c>
       <c r="P19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="Q19" s="124" t="s">
-        <v>156</v>
-      </c>
-      <c r="R19" s="124" t="s">
-        <v>157</v>
-      </c>
-      <c r="S19" s="124" t="s">
-        <v>158</v>
-      </c>
-      <c r="T19" s="124" t="s">
-        <v>219</v>
-      </c>
-      <c r="U19" s="124" t="s">
-        <v>159</v>
+      <c r="Q19" s="105">
+        <v>8</v>
+      </c>
+      <c r="R19" s="108" t="s">
+        <v>142</v>
+      </c>
+      <c r="S19" s="106" t="s">
+        <v>143</v>
+      </c>
+      <c r="T19" s="107" t="s">
+        <v>230</v>
+      </c>
+      <c r="U19" s="106" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -3228,54 +3214,52 @@
         <v>122</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>175</v>
+        <v>206</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="28" t="s">
-        <v>221</v>
+      <c r="G20" s="13" t="s">
+        <v>214</v>
       </c>
       <c r="H20" s="14">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J20" s="29" t="s">
-        <v>222</v>
-      </c>
-      <c r="K20" s="14" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="J20" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="K20" s="34" t="s">
+        <v>154</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M20" s="19"/>
-      <c r="N20" s="7" t="s">
-        <v>83</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="M20" s="35"/>
+      <c r="N20" s="19"/>
       <c r="O20" s="100" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q20" s="22">
-        <v>8</v>
+        <v>124</v>
+      </c>
+      <c r="Q20" s="22" t="s">
+        <v>156</v>
       </c>
       <c r="R20" s="23" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="S20" s="24" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="T20" s="25" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="U20" s="24" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -3289,23 +3273,23 @@
         <v>122</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>175</v>
+        <v>206</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="28" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="H21" s="14">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I21" s="18" t="s">
         <v>131</v>
       </c>
       <c r="J21" s="29" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="K21" s="14" t="s">
         <v>127</v>
@@ -3314,29 +3298,29 @@
         <v>140</v>
       </c>
       <c r="M21" s="19"/>
-      <c r="N21" s="7" t="s">
-        <v>100</v>
+      <c r="N21" s="19" t="s">
+        <v>97</v>
       </c>
       <c r="O21" s="100" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q21" s="22">
-        <v>8</v>
-      </c>
-      <c r="R21" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="S21" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T21" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="U21" s="24" t="s">
-        <v>145</v>
+        <v>124</v>
+      </c>
+      <c r="Q21" s="110" t="s">
+        <v>156</v>
+      </c>
+      <c r="R21" s="110" t="s">
+        <v>157</v>
+      </c>
+      <c r="S21" s="110" t="s">
+        <v>158</v>
+      </c>
+      <c r="T21" s="110" t="s">
+        <v>217</v>
+      </c>
+      <c r="U21" s="110" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -3350,23 +3334,23 @@
         <v>122</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
       <c r="E22" s="32" t="s">
         <v>175</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="28" t="s">
-        <v>230</v>
+        <v>337</v>
       </c>
       <c r="H22" s="14">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I22" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J22" s="33" t="s">
-        <v>231</v>
+      <c r="J22" s="29" t="s">
+        <v>219</v>
       </c>
       <c r="K22" s="14" t="s">
         <v>127</v>
@@ -3375,11 +3359,11 @@
         <v>140</v>
       </c>
       <c r="M22" s="19"/>
-      <c r="N22" s="19" t="s">
-        <v>104</v>
+      <c r="N22" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="O22" s="100" t="s">
-        <v>232</v>
+        <v>331</v>
       </c>
       <c r="P22" s="19" t="s">
         <v>124</v>
@@ -3394,14 +3378,14 @@
         <v>143</v>
       </c>
       <c r="T22" s="25" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="U22" s="24" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="26" t="s">
         <v>120</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -3410,37 +3394,37 @@
       <c r="C23" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="37" t="s">
-        <v>234</v>
+      <c r="D23" s="27" t="s">
+        <v>221</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>235</v>
+        <v>175</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="18" t="s">
-        <v>236</v>
+      <c r="G23" s="28" t="s">
+        <v>222</v>
       </c>
       <c r="H23" s="14">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I23" s="18" t="s">
         <v>131</v>
       </c>
       <c r="J23" s="29" t="s">
-        <v>237</v>
-      </c>
-      <c r="K23" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="K23" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="L23" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="N23" s="20"/>
+      <c r="L23" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="M23" s="19"/>
+      <c r="N23" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="O23" s="100" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="P23" s="19" t="s">
         <v>131</v>
@@ -3449,20 +3433,20 @@
         <v>8</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="S23" s="24" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="T23" s="25" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="U23" s="24" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="26" t="s">
         <v>120</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -3471,55 +3455,55 @@
       <c r="C24" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="37" t="s">
-        <v>241</v>
+      <c r="D24" s="27" t="s">
+        <v>226</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>235</v>
+        <v>175</v>
       </c>
       <c r="F24" s="4"/>
-      <c r="G24" s="18" t="s">
-        <v>191</v>
+      <c r="G24" s="28" t="s">
+        <v>227</v>
       </c>
       <c r="H24" s="14">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I24" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J24" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="K24" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="L24" s="15" t="s">
+      <c r="J24" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="L24" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="M24" s="20"/>
-      <c r="N24" s="7" t="s">
-        <v>103</v>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="O24" s="100" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="P24" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q24" s="22" t="s">
-        <v>189</v>
+        <v>131</v>
+      </c>
+      <c r="Q24" s="22">
+        <v>8</v>
       </c>
       <c r="R24" s="23" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="S24" s="24" t="s">
-        <v>190</v>
+        <v>143</v>
       </c>
       <c r="T24" s="25" t="s">
-        <v>191</v>
+        <v>339</v>
       </c>
       <c r="U24" s="24" t="s">
-        <v>192</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -3533,36 +3517,36 @@
         <v>122</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="18" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="H25" s="14">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>131</v>
       </c>
       <c r="J25" s="29" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="K25" s="39" t="s">
         <v>127</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="M25" s="20"/>
-      <c r="N25" s="7" t="s">
-        <v>97</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="N25" s="20"/>
       <c r="O25" s="100" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="P25" s="19" t="s">
         <v>124</v>
@@ -3571,16 +3555,16 @@
         <v>8</v>
       </c>
       <c r="R25" s="23" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="S25" s="24" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="U25" s="24" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -3594,41 +3578,55 @@
         <v>122</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E26" s="32" t="s">
-        <v>10</v>
+        <v>232</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="18" t="s">
-        <v>10</v>
+        <v>190</v>
       </c>
       <c r="H26" s="14">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I26" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J26" s="41" t="s">
-        <v>248</v>
-      </c>
-      <c r="K26" s="39" t="s">
-        <v>127</v>
+      <c r="J26" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="K26" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="L26" s="15" t="s">
-        <v>249</v>
+        <v>140</v>
       </c>
       <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
+      <c r="N26" s="7" t="s">
+        <v>103</v>
+      </c>
       <c r="O26" s="100" t="s">
-        <v>250</v>
-      </c>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="46"/>
-      <c r="U26" s="45"/>
+        <v>240</v>
+      </c>
+      <c r="P26" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q26" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="R26" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="S26" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="T26" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="U26" s="24" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="36" t="s">
@@ -3640,24 +3638,24 @@
       <c r="C27" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="47" t="s">
-        <v>241</v>
+      <c r="D27" s="37" t="s">
+        <v>238</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="18" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="H27" s="14">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I27" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J27" s="16" t="s">
-        <v>253</v>
+      <c r="J27" s="29" t="s">
+        <v>242</v>
       </c>
       <c r="K27" s="39" t="s">
         <v>127</v>
@@ -3665,12 +3663,12 @@
       <c r="L27" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="M27" s="48"/>
+      <c r="M27" s="20"/>
       <c r="N27" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="O27" s="99" t="s">
-        <v>255</v>
+        <v>97</v>
+      </c>
+      <c r="O27" s="100" t="s">
+        <v>243</v>
       </c>
       <c r="P27" s="19" t="s">
         <v>124</v>
@@ -3679,13 +3677,13 @@
         <v>8</v>
       </c>
       <c r="R27" s="23" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="S27" s="24" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="T27" s="25" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="U27" s="24" t="s">
         <v>145</v>
@@ -3701,122 +3699,182 @@
       <c r="C28" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="47" t="s">
-        <v>241</v>
+      <c r="D28" s="37" t="s">
+        <v>238</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>257</v>
+        <v>10</v>
       </c>
       <c r="F28" s="4"/>
-      <c r="G28" s="18"/>
+      <c r="G28" s="18" t="s">
+        <v>10</v>
+      </c>
       <c r="H28" s="14">
+        <v>24</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="K28" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="100" t="s">
+        <v>247</v>
+      </c>
+      <c r="P28" s="42"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="44"/>
+      <c r="S28" s="45"/>
+      <c r="T28" s="46"/>
+      <c r="U28" s="45"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="H29" s="14">
+        <v>25</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="K29" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="L29" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="M29" s="48"/>
+      <c r="N29" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="O29" s="99" t="s">
+        <v>252</v>
+      </c>
+      <c r="P29" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q29" s="22">
+        <v>8</v>
+      </c>
+      <c r="R29" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="S29" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="T29" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="U29" s="24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="14">
         <v>26</v>
       </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="48"/>
-      <c r="O28" s="99"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="53"/>
-      <c r="U28" s="52"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="63"/>
-      <c r="L29" s="62"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="64"/>
-      <c r="O29" s="101"/>
-      <c r="P29" s="66"/>
-      <c r="Q29" s="65"/>
-      <c r="R29" s="67"/>
-      <c r="S29" s="68"/>
-      <c r="T29" s="69"/>
-      <c r="U29" s="68"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
-      <c r="B30" s="70"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="76"/>
-      <c r="K30" s="63"/>
-      <c r="L30" s="62"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="64"/>
-      <c r="O30" s="102"/>
-      <c r="P30" s="78"/>
-      <c r="Q30" s="77"/>
-      <c r="R30" s="79"/>
-      <c r="S30" s="80"/>
-      <c r="T30" s="81"/>
-      <c r="U30" s="80"/>
-    </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="82"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="83"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="99"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="52"/>
+      <c r="T30" s="53"/>
+      <c r="U30" s="52"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="54"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="55"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="87"/>
-      <c r="I31" s="88"/>
-      <c r="J31" s="89"/>
-      <c r="K31" s="91"/>
-      <c r="L31" s="90"/>
-      <c r="M31" s="92"/>
-      <c r="N31" s="92"/>
-      <c r="O31" s="103"/>
-      <c r="P31" s="94"/>
-      <c r="Q31" s="93"/>
-      <c r="R31" s="95"/>
-      <c r="S31" s="96"/>
-      <c r="T31" s="97"/>
-      <c r="U31" s="96"/>
-    </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="82"/>
-      <c r="B32" s="83"/>
-      <c r="C32" s="84"/>
-      <c r="D32" s="85"/>
-      <c r="E32" s="83"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="62"/>
+      <c r="M31" s="64"/>
+      <c r="N31" s="64"/>
+      <c r="O31" s="101"/>
+      <c r="P31" s="66"/>
+      <c r="Q31" s="65"/>
+      <c r="R31" s="67"/>
+      <c r="S31" s="68"/>
+      <c r="T31" s="69"/>
+      <c r="U31" s="68"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="54"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="70"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="86"/>
-      <c r="H32" s="87"/>
-      <c r="I32" s="88"/>
-      <c r="J32" s="89"/>
-      <c r="K32" s="91"/>
-      <c r="L32" s="90"/>
-      <c r="M32" s="92"/>
-      <c r="N32" s="92"/>
-      <c r="O32" s="103"/>
-      <c r="P32" s="94"/>
-      <c r="Q32" s="93"/>
-      <c r="R32" s="95"/>
-      <c r="S32" s="96"/>
-      <c r="T32" s="97"/>
-      <c r="U32" s="96"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="76"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="102"/>
+      <c r="P32" s="78"/>
+      <c r="Q32" s="77"/>
+      <c r="R32" s="79"/>
+      <c r="S32" s="80"/>
+      <c r="T32" s="81"/>
+      <c r="U32" s="80"/>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="82"/>
@@ -3887,168 +3945,205 @@
       <c r="T35" s="97"/>
       <c r="U35" s="96"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="82"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="83"/>
       <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>258</v>
-      </c>
-      <c r="C37" t="s">
-        <v>120</v>
-      </c>
-      <c r="D37" t="s">
-        <v>259</v>
-      </c>
-      <c r="E37" t="s">
-        <v>260</v>
-      </c>
+      <c r="G36" s="86"/>
+      <c r="H36" s="87"/>
+      <c r="I36" s="88"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="91"/>
+      <c r="L36" s="90"/>
+      <c r="M36" s="92"/>
+      <c r="N36" s="92"/>
+      <c r="O36" s="103"/>
+      <c r="P36" s="94"/>
+      <c r="Q36" s="93"/>
+      <c r="R36" s="95"/>
+      <c r="S36" s="96"/>
+      <c r="T36" s="97"/>
+      <c r="U36" s="96"/>
+    </row>
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="82"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="83"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="98" t="s">
-        <v>261</v>
-      </c>
+      <c r="G37" s="86"/>
+      <c r="H37" s="87"/>
+      <c r="I37" s="88"/>
+      <c r="J37" s="89"/>
+      <c r="K37" s="91"/>
+      <c r="L37" s="90"/>
+      <c r="M37" s="92"/>
+      <c r="N37" s="92"/>
+      <c r="O37" s="103"/>
+      <c r="P37" s="94"/>
+      <c r="Q37" s="93"/>
+      <c r="R37" s="95"/>
+      <c r="S37" s="96"/>
+      <c r="T37" s="97"/>
+      <c r="U37" s="96"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>262</v>
-      </c>
-      <c r="C38" t="s">
-        <v>127</v>
-      </c>
-      <c r="D38" t="s">
-        <v>154</v>
-      </c>
       <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C39" t="s">
-        <v>264</v>
+        <v>120</v>
       </c>
       <c r="D39" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="E39" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="98" t="s">
-        <v>128</v>
-      </c>
-      <c r="J39" t="s">
-        <v>140</v>
-      </c>
-      <c r="K39" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>267</v>
+        <v>258</v>
+      </c>
+      <c r="C40" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" t="s">
+        <v>154</v>
       </c>
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>268</v>
+        <v>259</v>
+      </c>
+      <c r="C41" t="s">
+        <v>260</v>
+      </c>
+      <c r="D41" t="s">
+        <v>261</v>
+      </c>
+      <c r="E41" t="s">
+        <v>262</v>
       </c>
       <c r="F41" s="4"/>
+      <c r="G41" s="98" t="s">
+        <v>128</v>
+      </c>
+      <c r="J41" t="s">
+        <v>140</v>
+      </c>
+      <c r="K41" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>187</v>
-      </c>
-      <c r="E43" t="s">
-        <v>126</v>
+        <v>264</v>
       </c>
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>270</v>
-      </c>
-      <c r="E44" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>271</v>
+        <v>186</v>
       </c>
       <c r="E45" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E46" t="s">
-        <v>170</v>
+        <v>251</v>
       </c>
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>267</v>
       </c>
       <c r="E47" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>273</v>
+        <v>268</v>
+      </c>
+      <c r="E48" t="s">
+        <v>170</v>
       </c>
       <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>274</v>
+        <v>129</v>
+      </c>
+      <c r="E49" t="s">
+        <v>139</v>
       </c>
       <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>238</v>
+        <v>271</v>
       </c>
       <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>210</v>
+        <v>272</v>
       </c>
       <c r="F53" s="4"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>235</v>
+      </c>
       <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>277</v>
+        <v>208</v>
       </c>
       <c r="F55" s="4"/>
     </row>
@@ -4056,6 +4151,9 @@
       <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>273</v>
+      </c>
       <c r="F57" s="4"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -4097,480 +4195,484 @@
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F70" s="4"/>
     </row>
-    <row r="72" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F71" s="4"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F72" s="4"/>
+    </row>
     <row r="74" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>86</v>
-      </c>
-      <c r="C76" t="s">
-        <v>87</v>
-      </c>
-      <c r="E76" t="s">
-        <v>88</v>
-      </c>
-      <c r="J76" t="s">
-        <v>89</v>
-      </c>
-      <c r="L76" t="s">
-        <v>90</v>
-      </c>
-    </row>
+    <row r="76" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>94</v>
-      </c>
-    </row>
+        <v>86</v>
+      </c>
+      <c r="C78" t="s">
+        <v>87</v>
+      </c>
+      <c r="E78" t="s">
+        <v>88</v>
+      </c>
+      <c r="J78" t="s">
+        <v>89</v>
+      </c>
+      <c r="L78" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="80" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>278</v>
+        <v>84</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>279</v>
+        <v>85</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>328</v>
+      </c>
+    </row>
     <row r="170" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="171" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="172" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4686,11 +4788,19 @@
     <row r="282" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="283" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="284" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:U2">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4705,28 +4815,22 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L35">
-      <formula1>$C$39:$L$39</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L37">
+      <formula1>$C$41:$L$41</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K35">
-      <formula1>$C$38:$D$38</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K37">
+      <formula1>$C$40:$D$40</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A35">
-      <formula1>$C$37:$F$37</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A37">
+      <formula1>$C$39:$F$39</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3 M7 M5 M20:M21 M23:M35 N18 M10 M15 N16 N12">
-      <formula1>$A$41:$A$53</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3 M7 M5 M22:M23 M25:M37 N20 M11 M16 N17 N13">
+      <formula1>$A$43:$A$55</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3 N7 N5 N10 N15 N20:N21 N23:N35">
-      <formula1>$A$78:$A$167</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3 N7 N5 N11 N16 N22:N23 N25:N37">
+      <formula1>$A$80:$A$169</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Escaleta math 8 tema 2
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
@@ -22,90 +22,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Edgar Josué Malagón Montaña</author>
-  </authors>
-  <commentList>
-    <comment ref="U9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Edgar Josué Malagón Montaña:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Revisar esta parte, este recurso no es aprovechado.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U20" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Edgar Josué Malagón Montaña:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Esto no se habia planteado por el autor, revisar que se utilice de forma adecuada.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q21" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Edgar Josué Malagón Montaña:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Revisar esta parte porque este recurso no es aprovechado, el autor lo construyo.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="353">
   <si>
     <t>Asignatura</t>
   </si>
@@ -489,9 +407,6 @@
     <t>COMUNICACIÓN</t>
   </si>
   <si>
-    <t xml:space="preserve">NUEVO </t>
-  </si>
-  <si>
     <t xml:space="preserve">INTERACTIVO </t>
   </si>
   <si>
@@ -558,9 +473,6 @@
     <t>Corresponde al REC20 del manuscrito original. Incluye una serie de enunciados en lenguaje natural, representados a partir de una imagen y se espera que el estudiante seleccione la respuesta correcta de la expresión en lenguaje algebraico que modele la situación.</t>
   </si>
   <si>
-    <t>Recurso M7A-01</t>
-  </si>
-  <si>
     <t>Polinomios</t>
   </si>
   <si>
@@ -570,9 +482,6 @@
     <t>Actividad que muestra los conceptos básicos de los polinomios</t>
   </si>
   <si>
-    <t xml:space="preserve">APROVECHADO </t>
-  </si>
-  <si>
     <t>Corresponde al REC30 del manuscrito original. Se propone en este orden, debido a que en este recurso se pretende que el estudiante complete un texto a partir de términos claves de los polinomios.</t>
   </si>
   <si>
@@ -736,9 +645,6 @@
   </si>
   <si>
     <t>La construcción del interactivo se realizará de la siguiente manera: en la diapositiva 1, se incluirá el ejemplo de división entre expresiones algebraicas que propone el autor en la IMG06; en la diapositiva 2 se incluirán con un color distinto los ejemplos de división de monomios; en la diapositiva 3 se incluirá el ejemplo propuesto por el autor de división de un polinomio por un monomio, pero se sugiere indicar con un color distinto la dvisión de cada término del polinomio por el monomio y el resultado del respectivo color; en la diapositiva 4 se incluirá la explicación del algoritmo de división entre dos polinomios y se pueden aprovechar como ejemplo la IMG07 o la IMG08 propuestas por el autor en el manuscrito.</t>
-  </si>
-  <si>
-    <t>Recurso F13B-02</t>
   </si>
   <si>
     <t>Practica la división de polinomios</t>
@@ -815,12 +721,6 @@
     <t>Recurso M5A-01</t>
   </si>
   <si>
-    <t>Cercitación y competencias</t>
-  </si>
-  <si>
-    <t>Fin de la unidad</t>
-  </si>
-  <si>
     <t xml:space="preserve">Competencias: el proceso de la construcción del álgebra </t>
   </si>
   <si>
@@ -836,9 +736,6 @@
     <t>Recurso F13-01</t>
   </si>
   <si>
-    <t>Ejercitación y competencias</t>
-  </si>
-  <si>
     <t>Esta actividad permite ejercitar las operaciones básicas con los polinomios</t>
   </si>
   <si>
@@ -866,9 +763,6 @@
     <t>Correpsonde al REC220 propuesto por el autor.</t>
   </si>
   <si>
-    <t>Autoevaluación</t>
-  </si>
-  <si>
     <t>Evaluación</t>
   </si>
   <si>
@@ -881,9 +775,6 @@
     <t>Corresponde al REC230 propuesto por el autor. Se propone un test matemático que incluye diversas situaciones problema, con el objeto de seleccionar la respuesta apropiada.</t>
   </si>
   <si>
-    <t>Webs de referencia</t>
-  </si>
-  <si>
     <t>ASIGNATURA</t>
   </si>
   <si>
@@ -1121,9 +1012,6 @@
     <t>Este interactivo permitirá que el estudiante descubra por qué es válido el teorema del residuo. Se pueden utilizar los ejercicios que planteo el autor en el REC150</t>
   </si>
   <si>
-    <t>Recurso M101-01</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Las operaciones aditivas entre polinomios</t>
   </si>
   <si>
@@ -1152,13 +1040,70 @@
   </si>
   <si>
     <t>Recurso M5A-03</t>
+  </si>
+  <si>
+    <t>Competencias</t>
+  </si>
+  <si>
+    <t>Fin de tema</t>
+  </si>
+  <si>
+    <t>Banco de contenidos</t>
+  </si>
+  <si>
+    <t>Secuencia de imágenes que repasa los conceptos básicos del álgebra</t>
+  </si>
+  <si>
+    <t>Practica las operaciones con expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Recurso M7A-02</t>
+  </si>
+  <si>
+    <t>Recurso M%A-01</t>
+  </si>
+  <si>
+    <t>Recurso M101A-01</t>
+  </si>
+  <si>
+    <t>Recurso F13-02</t>
+  </si>
+  <si>
+    <t>Diaporama F1</t>
+  </si>
+  <si>
+    <t>Recursos M aleatorios y diaporama F1</t>
+  </si>
+  <si>
+    <t>Diaporama F1-01</t>
+  </si>
+  <si>
+    <t>RM_01_02_CO</t>
+  </si>
+  <si>
+    <t>Construir una secuencia de imágenes en la cual se explique el proceso para dividir polinomios y se sugieran actividades</t>
+  </si>
+  <si>
+    <t>Recurso M101AP-01</t>
+  </si>
+  <si>
+    <t>RM_01_01_CO</t>
+  </si>
+  <si>
+    <t>Practica la división de monomios</t>
+  </si>
+  <si>
+    <t>Actividad para practicar la división entre monomios</t>
+  </si>
+  <si>
+    <t>Ejercicios de practica de las operaciones con expresiones algebraicas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1222,19 +1167,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="8"/>
       <color theme="1"/>
@@ -1242,8 +1174,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1346,14 +1286,8 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1469,11 +1403,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1516,9 +1461,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1526,9 +1468,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1591,25 +1530,10 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1712,11 +1636,32 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1763,22 +1708,46 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2084,12 +2053,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U286"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T29" sqref="T29"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,20 +2069,20 @@
     <col min="4" max="4" width="45.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="30.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" style="98" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="98" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="77.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="91" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="91" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="77.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
     <col min="13" max="14" width="7.85546875" customWidth="1"/>
-    <col min="15" max="15" width="43" style="104" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15" customWidth="1"/>
+    <col min="15" max="15" width="43" style="97" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
+    <col min="19" max="19" width="20.85546875" customWidth="1"/>
+    <col min="20" max="20" width="31" customWidth="1"/>
+    <col min="21" max="21" width="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="6" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2160,22 +2129,22 @@
       <c r="O1" s="116" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="127" t="s">
+      <c r="P1" s="108" t="s">
         <v>119</v>
       </c>
-      <c r="Q1" s="127" t="s">
+      <c r="Q1" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="130" t="s">
+      <c r="R1" s="111" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="128" t="s">
+      <c r="S1" s="109" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="129" t="s">
+      <c r="T1" s="110" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="128" t="s">
+      <c r="U1" s="109" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2199,12 +2168,12 @@
         <v>92</v>
       </c>
       <c r="O2" s="116"/>
-      <c r="P2" s="127"/>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="130"/>
-      <c r="S2" s="128"/>
-      <c r="T2" s="129"/>
-      <c r="U2" s="128"/>
+      <c r="P2" s="108"/>
+      <c r="Q2" s="108"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="109"/>
+      <c r="T2" s="110"/>
+      <c r="U2" s="109"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -2224,7 +2193,7 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="13" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="H3" s="14">
         <v>1</v>
@@ -2236,39 +2205,39 @@
         <v>125</v>
       </c>
       <c r="K3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="L3" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="M3" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="N3" s="19"/>
+      <c r="O3" s="92" t="s">
         <v>129</v>
       </c>
-      <c r="N3" s="20"/>
-      <c r="O3" s="99" t="s">
-        <v>130</v>
-      </c>
-      <c r="P3" s="19" t="s">
+      <c r="P3" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="Q3" s="22">
+      <c r="Q3" s="20">
         <v>8</v>
       </c>
-      <c r="R3" s="23" t="s">
+      <c r="R3" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="S3" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="S3" s="24" t="s">
+      <c r="T3" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="T3" s="25" t="s">
+      <c r="U3" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="U3" s="24" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -2277,59 +2246,59 @@
       <c r="C4" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="25" t="s">
         <v>123</v>
       </c>
       <c r="E4" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="26" t="s">
         <v>136</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="28" t="s">
-        <v>137</v>
       </c>
       <c r="H4" s="14">
         <v>2</v>
       </c>
-      <c r="I4" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J4" s="29" t="s">
-        <v>138</v>
+      <c r="I4" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L4" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M4" s="28"/>
+      <c r="N4" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="O4" s="92" t="s">
         <v>140</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="O4" s="99" t="s">
+      <c r="P4" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q4" s="20">
+        <v>8</v>
+      </c>
+      <c r="R4" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="P4" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q4" s="22">
-        <v>8</v>
-      </c>
-      <c r="R4" s="23" t="s">
+      <c r="S4" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="T4" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="U4" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="U4" s="24" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="29" t="s">
         <v>120</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -2338,59 +2307,59 @@
       <c r="C5" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="25" t="s">
         <v>123</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H5" s="14">
         <v>3</v>
       </c>
-      <c r="I5" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>147</v>
+      <c r="I5" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>146</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M5" s="19"/>
+        <v>130</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M5" s="18"/>
       <c r="N5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="O5" s="99" t="s">
-        <v>149</v>
-      </c>
-      <c r="P5" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="O5" s="92" t="s">
+        <v>148</v>
+      </c>
+      <c r="P5" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="Q5" s="22">
+      <c r="Q5" s="20">
         <v>8</v>
       </c>
-      <c r="R5" s="23" t="s">
+      <c r="R5" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="S5" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="S5" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T5" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="U5" s="24" t="s">
-        <v>145</v>
+      <c r="T5" s="23" t="s">
+        <v>340</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -2399,59 +2368,59 @@
       <c r="C6" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="25" t="s">
         <v>123</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="28" t="s">
-        <v>152</v>
+      <c r="G6" s="26" t="s">
+        <v>150</v>
       </c>
       <c r="H6" s="14">
         <v>4</v>
       </c>
-      <c r="I6" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J6" s="29" t="s">
+      <c r="I6" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="O6" s="93" t="s">
+        <v>152</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q6" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="R6" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="L6" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="O6" s="100" t="s">
+      <c r="S6" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="P6" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q6" s="22" t="s">
+      <c r="T6" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="U6" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="R6" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="S6" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="T6" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="U6" s="24" t="s">
-        <v>159</v>
-      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -2460,59 +2429,59 @@
       <c r="C7" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="25" t="s">
         <v>123</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="28" t="s">
-        <v>160</v>
+      <c r="G7" s="26" t="s">
+        <v>157</v>
       </c>
       <c r="H7" s="14">
         <v>5</v>
       </c>
-      <c r="I7" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>161</v>
+      <c r="I7" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>158</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L7" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M7" s="19"/>
+        <v>130</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M7" s="18"/>
       <c r="N7" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="O7" s="100" t="s">
-        <v>162</v>
-      </c>
-      <c r="P7" s="19" t="s">
+      <c r="O7" s="93" t="s">
+        <v>159</v>
+      </c>
+      <c r="P7" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="Q7" s="20">
         <v>8</v>
       </c>
-      <c r="R7" s="23" t="s">
+      <c r="R7" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="S7" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="S7" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T7" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="U7" s="24" t="s">
-        <v>145</v>
+      <c r="T7" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="U7" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -2521,59 +2490,59 @@
       <c r="C8" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="25" t="s">
         <v>123</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="28" t="s">
-        <v>164</v>
+      <c r="G8" s="26" t="s">
+        <v>161</v>
       </c>
       <c r="H8" s="14">
         <v>6</v>
       </c>
-      <c r="I8" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>165</v>
+      <c r="I8" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>162</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L8" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="O8" s="100" t="s">
-        <v>166</v>
-      </c>
-      <c r="P8" s="19" t="s">
+      <c r="O8" s="93" t="s">
+        <v>163</v>
+      </c>
+      <c r="P8" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="Q8" s="20">
         <v>8</v>
       </c>
-      <c r="R8" s="23" t="s">
+      <c r="R8" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="S8" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="S8" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T8" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="U8" s="24" t="s">
-        <v>145</v>
+      <c r="T8" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="U8" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -2582,98 +2551,114 @@
       <c r="C9" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="25" t="s">
         <v>123</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="28" t="s">
-        <v>168</v>
+      <c r="G9" s="26" t="s">
+        <v>165</v>
       </c>
       <c r="H9" s="14">
         <v>7</v>
       </c>
-      <c r="I9" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J9" s="29" t="s">
+      <c r="I9" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="93" t="s">
+        <v>320</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q9" s="127" t="s">
+        <v>168</v>
+      </c>
+      <c r="R9" s="128" t="s">
+        <v>154</v>
+      </c>
+      <c r="S9" s="129" t="s">
         <v>169</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="T9" s="130" t="s">
+        <v>170</v>
+      </c>
+      <c r="U9" s="129" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="102"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="H10" s="14">
+        <v>8</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="L10" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="L9" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="111" t="s">
-        <v>329</v>
-      </c>
-      <c r="P9" s="110" t="s">
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="93" t="s">
+        <v>330</v>
+      </c>
+      <c r="P10" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="Q9" s="131" t="s">
+      <c r="Q10" s="127" t="s">
+        <v>168</v>
+      </c>
+      <c r="R10" s="128" t="s">
+        <v>154</v>
+      </c>
+      <c r="S10" s="129" t="s">
+        <v>169</v>
+      </c>
+      <c r="T10" s="130" t="s">
+        <v>331</v>
+      </c>
+      <c r="U10" s="129" t="s">
         <v>171</v>
       </c>
-      <c r="R9" s="131" t="s">
-        <v>157</v>
-      </c>
-      <c r="S9" s="131" t="s">
-        <v>172</v>
-      </c>
-      <c r="T9" s="131" t="s">
-        <v>173</v>
-      </c>
-      <c r="U9" s="131" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="28" t="s">
-        <v>341</v>
-      </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="111" t="s">
-        <v>340</v>
-      </c>
-      <c r="P10" s="110" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q10" s="132" t="s">
-        <v>171</v>
-      </c>
-      <c r="R10" s="132" t="s">
-        <v>157</v>
-      </c>
-      <c r="S10" s="132" t="s">
-        <v>172</v>
-      </c>
-      <c r="T10" s="132" t="s">
-        <v>341</v>
-      </c>
-      <c r="U10" s="132" t="s">
-        <v>174</v>
-      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2682,59 +2667,59 @@
       <c r="C11" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="E11" s="32" t="s">
-        <v>175</v>
+      <c r="E11" s="30" t="s">
+        <v>172</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="28" t="s">
-        <v>177</v>
+      <c r="G11" s="26" t="s">
+        <v>174</v>
       </c>
       <c r="H11" s="14">
-        <v>8</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>176</v>
+        <v>9</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>173</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L11" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M11" s="19"/>
+        <v>130</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M11" s="18"/>
       <c r="N11" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="O11" s="100" t="s">
-        <v>330</v>
-      </c>
-      <c r="P11" s="19" t="s">
+      <c r="O11" s="93" t="s">
+        <v>321</v>
+      </c>
+      <c r="P11" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="Q11" s="105">
+      <c r="Q11" s="98">
         <v>8</v>
       </c>
-      <c r="R11" s="108" t="s">
+      <c r="R11" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="S11" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="S11" s="106" t="s">
-        <v>143</v>
-      </c>
-      <c r="T11" s="107" t="s">
-        <v>333</v>
-      </c>
-      <c r="U11" s="106" t="s">
-        <v>145</v>
+      <c r="T11" s="100" t="s">
+        <v>341</v>
+      </c>
+      <c r="U11" s="99" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -2743,59 +2728,59 @@
       <c r="C12" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12" s="14">
+        <v>10</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J12" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="K12" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="O12" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="28" t="s">
+      <c r="P12" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q12" s="20">
+        <v>8</v>
+      </c>
+      <c r="R12" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="S12" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="T12" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="H12" s="14">
-        <v>9</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="O12" s="100" t="s">
-        <v>182</v>
-      </c>
-      <c r="P12" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q12" s="22">
-        <v>8</v>
-      </c>
-      <c r="R12" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="S12" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T12" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="U12" s="24" t="s">
-        <v>145</v>
+      <c r="U12" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -2804,59 +2789,59 @@
       <c r="C13" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D13" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>179</v>
+      <c r="D13" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>176</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="H13" s="14">
+        <v>11</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="N13" s="18"/>
+      <c r="O13" s="93" t="s">
         <v>184</v>
       </c>
-      <c r="H13" s="14">
-        <v>10</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="J13" s="29" t="s">
+      <c r="P13" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q13" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="R13" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="L13" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="M13" s="19" t="s">
+      <c r="S13" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="N13" s="19"/>
-      <c r="O13" s="100" t="s">
+      <c r="T13" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="P13" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q13" s="22" t="s">
+      <c r="U13" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="R13" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="S13" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="T13" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="U13" s="24" t="s">
-        <v>191</v>
-      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -2865,59 +2850,59 @@
       <c r="C14" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="E14" s="32" t="s">
+      <c r="D14" s="25" t="s">
         <v>175</v>
       </c>
+      <c r="E14" s="30" t="s">
+        <v>172</v>
+      </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="28" t="s">
-        <v>334</v>
+      <c r="G14" s="26" t="s">
+        <v>324</v>
       </c>
       <c r="H14" s="14">
-        <v>11</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J14" s="29" t="s">
-        <v>192</v>
+        <v>12</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>189</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L14" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="O14" s="100" t="s">
-        <v>193</v>
-      </c>
-      <c r="P14" s="19" t="s">
+      <c r="O14" s="93" t="s">
+        <v>190</v>
+      </c>
+      <c r="P14" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="Q14" s="22">
+      <c r="Q14" s="20">
         <v>8</v>
       </c>
-      <c r="R14" s="23" t="s">
+      <c r="R14" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="S14" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="S14" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T14" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="U14" s="24" t="s">
-        <v>145</v>
+      <c r="T14" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="U14" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -2926,59 +2911,59 @@
       <c r="C15" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="H15" s="14">
+        <v>13</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J15" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="K15" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="O15" s="93" t="s">
         <v>196</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="28" t="s">
+      <c r="P15" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q15" s="20">
+        <v>8</v>
+      </c>
+      <c r="R15" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="S15" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="T15" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="H15" s="14">
-        <v>12</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J15" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="K15" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L15" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="O15" s="100" t="s">
-        <v>199</v>
-      </c>
-      <c r="P15" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q15" s="22">
-        <v>8</v>
-      </c>
-      <c r="R15" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="S15" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T15" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="U15" s="24" t="s">
-        <v>145</v>
+      <c r="U15" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="29" t="s">
         <v>120</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -2987,59 +2972,59 @@
       <c r="C16" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>201</v>
+      <c r="D16" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>198</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="13" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H16" s="14">
-        <v>13</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J16" s="29" t="s">
-        <v>203</v>
+        <v>14</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J16" s="27" t="s">
+        <v>200</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L16" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M16" s="19"/>
+        <v>130</v>
+      </c>
+      <c r="L16" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M16" s="18"/>
       <c r="N16" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="O16" s="100" t="s">
-        <v>204</v>
-      </c>
-      <c r="P16" s="19" t="s">
+      <c r="O16" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="P16" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="Q16" s="22">
+      <c r="Q16" s="20">
         <v>8</v>
       </c>
-      <c r="R16" s="23" t="s">
+      <c r="R16" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="S16" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="S16" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T16" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="U16" s="24" t="s">
-        <v>145</v>
+      <c r="T16" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="U16" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -3048,59 +3033,59 @@
       <c r="C17" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="E17" s="32" t="s">
+      <c r="D17" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="14">
+        <v>15</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="M17" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="N17" s="18"/>
+      <c r="O17" s="93" t="s">
         <v>206</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="H17" s="14">
-        <v>14</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="K17" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L17" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="M17" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="N17" s="19"/>
-      <c r="O17" s="100" t="s">
-        <v>209</v>
-      </c>
-      <c r="P17" s="19" t="s">
+      <c r="P17" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q17" s="20">
+        <v>8</v>
+      </c>
+      <c r="R17" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="Q17" s="22">
-        <v>8</v>
-      </c>
-      <c r="R17" s="23" t="s">
+      <c r="S17" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="S17" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="T17" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="U17" s="24" t="s">
-        <v>135</v>
+      <c r="T17" s="23" t="s">
+        <v>342</v>
+      </c>
+      <c r="U17" s="22" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -3109,161 +3094,153 @@
       <c r="C18" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>206</v>
+      <c r="D18" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>203</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="13" t="s">
-        <v>211</v>
+        <v>350</v>
       </c>
       <c r="H18" s="14">
-        <v>15</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J18" s="29" t="s">
-        <v>212</v>
+        <v>16</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>351</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="L18" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="O18" s="100" t="s">
-        <v>213</v>
-      </c>
-      <c r="P18" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="Q18" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="R18" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="S18" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="T18" s="25" t="s">
-        <v>211</v>
-      </c>
-      <c r="U18" s="24" t="s">
-        <v>159</v>
+      <c r="L18" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18" s="93" t="s">
+        <v>209</v>
+      </c>
+      <c r="P18" s="131" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q18" s="104">
+        <v>8</v>
+      </c>
+      <c r="R18" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="S18" s="105" t="s">
+        <v>142</v>
+      </c>
+      <c r="T18" s="106" t="s">
+        <v>339</v>
+      </c>
+      <c r="U18" s="105" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="32"/>
+      <c r="D19" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E19" s="30"/>
       <c r="F19" s="4"/>
       <c r="G19" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="29" t="s">
-        <v>338</v>
+        <v>207</v>
+      </c>
+      <c r="H19" s="14">
+        <v>17</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>208</v>
       </c>
       <c r="K19" s="14"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="O19" s="100" t="s">
-        <v>342</v>
-      </c>
-      <c r="P19" s="19" t="s">
+      <c r="L19" s="17"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="93"/>
+      <c r="P19" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="Q19" s="105">
-        <v>8</v>
-      </c>
-      <c r="R19" s="108" t="s">
-        <v>142</v>
-      </c>
-      <c r="S19" s="106" t="s">
-        <v>143</v>
-      </c>
-      <c r="T19" s="107" t="s">
-        <v>230</v>
-      </c>
-      <c r="U19" s="106" t="s">
-        <v>145</v>
+      <c r="Q19" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="R19" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="S19" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="T19" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="U19" s="22" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>206</v>
-      </c>
+      <c r="A20" s="24"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E20" s="30"/>
       <c r="F20" s="4"/>
       <c r="G20" s="13" t="s">
-        <v>214</v>
+        <v>338</v>
       </c>
       <c r="H20" s="14">
-        <v>16</v>
-      </c>
-      <c r="I20" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J20" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="K20" s="14"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="N20" s="18"/>
+      <c r="O20" s="93" t="s">
+        <v>347</v>
+      </c>
+      <c r="P20" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="J20" s="33" t="s">
-        <v>215</v>
-      </c>
-      <c r="K20" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="L20" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="M20" s="35"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="100" t="s">
-        <v>332</v>
-      </c>
-      <c r="P20" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q20" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="R20" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="S20" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="T20" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="U20" s="24" t="s">
-        <v>159</v>
+      <c r="Q20" s="132">
+        <v>6</v>
+      </c>
+      <c r="R20" s="133" t="s">
+        <v>141</v>
+      </c>
+      <c r="S20" s="135" t="s">
+        <v>344</v>
+      </c>
+      <c r="T20" s="134" t="s">
+        <v>345</v>
+      </c>
+      <c r="U20" s="135" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -3272,59 +3249,57 @@
       <c r="C21" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>206</v>
-      </c>
+      <c r="D21" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E21" s="30"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="28" t="s">
-        <v>217</v>
+      <c r="G21" s="13" t="s">
+        <v>326</v>
       </c>
       <c r="H21" s="14">
-        <v>17</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>218</v>
+        <v>19</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>328</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L21" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="O21" s="100" t="s">
-        <v>218</v>
-      </c>
-      <c r="P21" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="O21" s="93" t="s">
+        <v>332</v>
+      </c>
+      <c r="P21" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="Q21" s="110" t="s">
-        <v>156</v>
-      </c>
-      <c r="R21" s="110" t="s">
-        <v>157</v>
-      </c>
-      <c r="S21" s="110" t="s">
-        <v>158</v>
-      </c>
-      <c r="T21" s="110" t="s">
-        <v>217</v>
-      </c>
-      <c r="U21" s="110" t="s">
-        <v>159</v>
+      <c r="Q21" s="98">
+        <v>8</v>
+      </c>
+      <c r="R21" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="S21" s="99" t="s">
+        <v>142</v>
+      </c>
+      <c r="T21" s="100" t="s">
+        <v>226</v>
+      </c>
+      <c r="U21" s="99" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B22" s="9" t="s">
@@ -3333,59 +3308,57 @@
       <c r="C22" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D22" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>175</v>
+      <c r="D22" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>203</v>
       </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="28" t="s">
-        <v>337</v>
+      <c r="G22" s="13" t="s">
+        <v>210</v>
       </c>
       <c r="H22" s="14">
-        <v>18</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J22" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="K22" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="J22" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="K22" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="L22" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="L22" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M22" s="19"/>
-      <c r="N22" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="O22" s="100" t="s">
-        <v>331</v>
-      </c>
-      <c r="P22" s="19" t="s">
+      <c r="M22" s="33"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="93" t="s">
+        <v>323</v>
+      </c>
+      <c r="P22" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="Q22" s="22">
-        <v>8</v>
-      </c>
-      <c r="R22" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="S22" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T22" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="U22" s="24" t="s">
-        <v>145</v>
+      <c r="Q22" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="R22" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="S22" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="T22" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="U22" s="22" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -3394,59 +3367,59 @@
       <c r="C23" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>175</v>
+      <c r="D23" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>203</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="28" t="s">
-        <v>222</v>
+      <c r="G23" s="26" t="s">
+        <v>213</v>
       </c>
       <c r="H23" s="14">
-        <v>19</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J23" s="29" t="s">
-        <v>223</v>
+        <v>21</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>214</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L23" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M23" s="19"/>
-      <c r="N23" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="O23" s="100" t="s">
-        <v>224</v>
-      </c>
-      <c r="P23" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q23" s="22">
-        <v>8</v>
-      </c>
-      <c r="R23" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="S23" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T23" s="25" t="s">
-        <v>225</v>
-      </c>
-      <c r="U23" s="24" t="s">
-        <v>145</v>
+        <v>130</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="O23" s="93" t="s">
+        <v>214</v>
+      </c>
+      <c r="P23" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q23" s="104" t="s">
+        <v>153</v>
+      </c>
+      <c r="R23" s="107" t="s">
+        <v>154</v>
+      </c>
+      <c r="S23" s="105" t="s">
+        <v>155</v>
+      </c>
+      <c r="T23" s="106" t="s">
+        <v>213</v>
+      </c>
+      <c r="U23" s="105" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -3455,59 +3428,59 @@
       <c r="C24" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>175</v>
+      <c r="D24" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>172</v>
       </c>
       <c r="F24" s="4"/>
-      <c r="G24" s="28" t="s">
-        <v>227</v>
+      <c r="G24" s="26" t="s">
+        <v>327</v>
       </c>
       <c r="H24" s="14">
-        <v>20</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J24" s="33" t="s">
-        <v>228</v>
+        <v>22</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="27" t="s">
+        <v>215</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L24" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="O24" s="100" t="s">
-        <v>229</v>
-      </c>
-      <c r="P24" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q24" s="22">
+        <v>130</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M24" s="18"/>
+      <c r="N24" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="O24" s="93" t="s">
+        <v>322</v>
+      </c>
+      <c r="P24" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q24" s="20">
         <v>8</v>
       </c>
-      <c r="R24" s="23" t="s">
+      <c r="R24" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="S24" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="S24" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T24" s="25" t="s">
-        <v>339</v>
-      </c>
-      <c r="U24" s="24" t="s">
-        <v>145</v>
+      <c r="T24" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="U24" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B25" s="9" t="s">
@@ -3516,59 +3489,59 @@
       <c r="C25" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="37" t="s">
-        <v>231</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>232</v>
+      <c r="D25" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>172</v>
       </c>
       <c r="F25" s="4"/>
-      <c r="G25" s="18" t="s">
-        <v>233</v>
+      <c r="G25" s="26" t="s">
+        <v>218</v>
       </c>
       <c r="H25" s="14">
-        <v>21</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J25" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="K25" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="L25" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="M25" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="N25" s="20"/>
-      <c r="O25" s="100" t="s">
-        <v>236</v>
-      </c>
-      <c r="P25" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q25" s="22">
+        <v>23</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M25" s="18"/>
+      <c r="N25" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O25" s="93" t="s">
+        <v>220</v>
+      </c>
+      <c r="P25" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q25" s="20">
         <v>8</v>
       </c>
-      <c r="R25" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="S25" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="T25" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="U25" s="24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
+      <c r="R25" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="S25" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="T25" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="U25" s="22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -3577,59 +3550,59 @@
       <c r="C26" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>232</v>
+      <c r="D26" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>172</v>
       </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="18" t="s">
-        <v>190</v>
+      <c r="G26" s="26" t="s">
+        <v>223</v>
       </c>
       <c r="H26" s="14">
-        <v>22</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J26" s="29" t="s">
-        <v>239</v>
-      </c>
-      <c r="K26" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="L26" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="M26" s="20"/>
-      <c r="N26" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="O26" s="100" t="s">
-        <v>240</v>
-      </c>
-      <c r="P26" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q26" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="R26" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="S26" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="T26" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="U26" s="24" t="s">
-        <v>191</v>
+        <v>24</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J26" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="O26" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="P26" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q26" s="20">
+        <v>8</v>
+      </c>
+      <c r="R26" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="S26" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="T26" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="U26" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="34" t="s">
         <v>120</v>
       </c>
       <c r="B27" s="9" t="s">
@@ -3638,59 +3611,57 @@
       <c r="C27" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="E27" s="32" t="s">
-        <v>232</v>
-      </c>
+      <c r="D27" s="35" t="s">
+        <v>334</v>
+      </c>
+      <c r="E27" s="30"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="18" t="s">
-        <v>241</v>
+      <c r="G27" s="17" t="s">
+        <v>227</v>
       </c>
       <c r="H27" s="14">
-        <v>23</v>
-      </c>
-      <c r="I27" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="L27" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="N27" s="19"/>
+      <c r="O27" s="93" t="s">
+        <v>230</v>
+      </c>
+      <c r="P27" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q27" s="20">
+        <v>8</v>
+      </c>
+      <c r="R27" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="J27" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="K27" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="L27" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="M27" s="20"/>
-      <c r="N27" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="O27" s="100" t="s">
-        <v>243</v>
-      </c>
-      <c r="P27" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q27" s="22">
-        <v>8</v>
-      </c>
-      <c r="R27" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="S27" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="T27" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="U27" s="24" t="s">
-        <v>145</v>
+      <c r="S27" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="T27" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="U27" s="22" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="34" t="s">
         <v>120</v>
       </c>
       <c r="B28" s="9" t="s">
@@ -3699,43 +3670,57 @@
       <c r="C28" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>10</v>
-      </c>
+      <c r="D28" s="35" t="s">
+        <v>334</v>
+      </c>
+      <c r="E28" s="30"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="14">
-        <v>24</v>
-      </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="41" t="s">
-        <v>245</v>
-      </c>
-      <c r="K28" s="39" t="s">
-        <v>127</v>
+      <c r="G28" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="H28" s="140">
+        <v>26</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J28" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="K28" s="38" t="s">
+        <v>124</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="100" t="s">
-        <v>247</v>
-      </c>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="43"/>
-      <c r="R28" s="44"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="46"/>
-      <c r="U28" s="45"/>
+        <v>139</v>
+      </c>
+      <c r="M28" s="19"/>
+      <c r="N28" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="O28" s="93" t="s">
+        <v>233</v>
+      </c>
+      <c r="P28" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q28" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="R28" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="S28" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="T28" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="U28" s="22" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="34" t="s">
         <v>120</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -3744,59 +3729,57 @@
       <c r="C29" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D29" s="47" t="s">
-        <v>238</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>248</v>
-      </c>
+      <c r="D29" s="35" t="s">
+        <v>334</v>
+      </c>
+      <c r="E29" s="30"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="H29" s="14">
-        <v>25</v>
-      </c>
-      <c r="I29" s="18" t="s">
+      <c r="G29" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="H29" s="140">
+        <v>27</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="K29" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="L29" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="M29" s="19"/>
+      <c r="N29" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O29" s="93" t="s">
+        <v>236</v>
+      </c>
+      <c r="P29" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="J29" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="K29" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="L29" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="M29" s="48"/>
-      <c r="N29" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="O29" s="99" t="s">
-        <v>252</v>
-      </c>
-      <c r="P29" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q29" s="22">
+      <c r="Q29" s="20">
         <v>8</v>
       </c>
-      <c r="R29" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="S29" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="T29" s="25" t="s">
-        <v>343</v>
-      </c>
-      <c r="U29" s="24" t="s">
-        <v>145</v>
+      <c r="R29" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="S29" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="T29" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="U29" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="34" t="s">
         <v>120</v>
       </c>
       <c r="B30" s="9" t="s">
@@ -3805,354 +3788,469 @@
       <c r="C30" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="14">
+        <v>28</v>
+      </c>
+      <c r="I30" s="17"/>
+      <c r="J30" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="E30" s="32" t="s">
-        <v>253</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="14">
-        <v>26</v>
-      </c>
-      <c r="I30" s="17"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="99"/>
-      <c r="P30" s="50"/>
-      <c r="Q30" s="21"/>
-      <c r="R30" s="51"/>
-      <c r="S30" s="52"/>
-      <c r="T30" s="53"/>
-      <c r="U30" s="52"/>
+      <c r="K30" s="103" t="s">
+        <v>130</v>
+      </c>
+      <c r="L30" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="93" t="s">
+        <v>240</v>
+      </c>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="42"/>
+      <c r="S30" s="43"/>
+      <c r="T30" s="44"/>
+      <c r="U30" s="43"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="55"/>
+      <c r="A31" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>241</v>
+      </c>
       <c r="F31" s="4"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="62"/>
-      <c r="M31" s="64"/>
-      <c r="N31" s="64"/>
-      <c r="O31" s="101"/>
-      <c r="P31" s="66"/>
-      <c r="Q31" s="65"/>
-      <c r="R31" s="67"/>
-      <c r="S31" s="68"/>
-      <c r="T31" s="69"/>
-      <c r="U31" s="68"/>
+      <c r="G31" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="H31" s="14">
+        <v>29</v>
+      </c>
+      <c r="I31" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="K31" s="103" t="s">
+        <v>130</v>
+      </c>
+      <c r="L31" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="M31" s="45"/>
+      <c r="N31" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="O31" s="92" t="s">
+        <v>244</v>
+      </c>
+      <c r="P31" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q31" s="104">
+        <v>8</v>
+      </c>
+      <c r="R31" s="107" t="s">
+        <v>131</v>
+      </c>
+      <c r="S31" s="105" t="s">
+        <v>132</v>
+      </c>
+      <c r="T31" s="106" t="s">
+        <v>333</v>
+      </c>
+      <c r="U31" s="105" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="70"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="70"/>
+      <c r="A32" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="E32" s="30"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="76"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="62"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="64"/>
-      <c r="O32" s="102"/>
-      <c r="P32" s="78"/>
-      <c r="Q32" s="77"/>
-      <c r="R32" s="79"/>
-      <c r="S32" s="80"/>
-      <c r="T32" s="81"/>
-      <c r="U32" s="80"/>
-    </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="82"/>
-      <c r="B33" s="83"/>
-      <c r="C33" s="84"/>
-      <c r="D33" s="85"/>
-      <c r="E33" s="83"/>
+      <c r="G32" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="H32" s="14">
+        <v>30</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J32" s="16"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="M32" s="45"/>
+      <c r="N32" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="O32" s="92"/>
+      <c r="P32" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q32" s="136">
+        <v>6</v>
+      </c>
+      <c r="R32" s="137" t="s">
+        <v>141</v>
+      </c>
+      <c r="S32" s="138" t="s">
+        <v>142</v>
+      </c>
+      <c r="T32" s="139" t="s">
+        <v>348</v>
+      </c>
+      <c r="U32" s="138" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="47"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="48"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="86"/>
-      <c r="H33" s="87"/>
-      <c r="I33" s="88"/>
-      <c r="J33" s="89"/>
-      <c r="K33" s="91"/>
-      <c r="L33" s="90"/>
-      <c r="M33" s="92"/>
-      <c r="N33" s="92"/>
-      <c r="O33" s="103"/>
-      <c r="P33" s="94"/>
-      <c r="Q33" s="93"/>
-      <c r="R33" s="95"/>
-      <c r="S33" s="96"/>
-      <c r="T33" s="97"/>
-      <c r="U33" s="96"/>
-    </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="82"/>
-      <c r="B34" s="83"/>
-      <c r="C34" s="84"/>
-      <c r="D34" s="85"/>
-      <c r="E34" s="83"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="57"/>
+      <c r="N33" s="57"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="59"/>
+      <c r="Q33" s="58"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="61"/>
+      <c r="T33" s="62"/>
+      <c r="U33" s="61"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="47"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="63"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="87"/>
-      <c r="I34" s="88"/>
-      <c r="J34" s="89"/>
-      <c r="K34" s="91"/>
-      <c r="L34" s="90"/>
-      <c r="M34" s="92"/>
-      <c r="N34" s="92"/>
-      <c r="O34" s="103"/>
-      <c r="P34" s="94"/>
-      <c r="Q34" s="93"/>
-      <c r="R34" s="95"/>
-      <c r="S34" s="96"/>
-      <c r="T34" s="97"/>
-      <c r="U34" s="96"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="68"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="56"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="57"/>
+      <c r="N34" s="57"/>
+      <c r="O34" s="95"/>
+      <c r="P34" s="71"/>
+      <c r="Q34" s="70"/>
+      <c r="R34" s="72"/>
+      <c r="S34" s="73"/>
+      <c r="T34" s="74"/>
+      <c r="U34" s="73"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="82"/>
-      <c r="B35" s="83"/>
-      <c r="C35" s="84"/>
-      <c r="D35" s="85"/>
-      <c r="E35" s="83"/>
+      <c r="A35" s="75"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="76"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="87"/>
-      <c r="I35" s="88"/>
-      <c r="J35" s="89"/>
-      <c r="K35" s="91"/>
-      <c r="L35" s="90"/>
-      <c r="M35" s="92"/>
-      <c r="N35" s="92"/>
-      <c r="O35" s="103"/>
-      <c r="P35" s="94"/>
-      <c r="Q35" s="93"/>
-      <c r="R35" s="95"/>
-      <c r="S35" s="96"/>
-      <c r="T35" s="97"/>
-      <c r="U35" s="96"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="82"/>
+      <c r="K35" s="84"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="85"/>
+      <c r="N35" s="85"/>
+      <c r="O35" s="96"/>
+      <c r="P35" s="87"/>
+      <c r="Q35" s="86"/>
+      <c r="R35" s="88"/>
+      <c r="S35" s="89"/>
+      <c r="T35" s="90"/>
+      <c r="U35" s="89"/>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="82"/>
-      <c r="B36" s="83"/>
-      <c r="C36" s="84"/>
-      <c r="D36" s="85"/>
-      <c r="E36" s="83"/>
+      <c r="A36" s="75"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="76"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="87"/>
-      <c r="I36" s="88"/>
-      <c r="J36" s="89"/>
-      <c r="K36" s="91"/>
-      <c r="L36" s="90"/>
-      <c r="M36" s="92"/>
-      <c r="N36" s="92"/>
-      <c r="O36" s="103"/>
-      <c r="P36" s="94"/>
-      <c r="Q36" s="93"/>
-      <c r="R36" s="95"/>
-      <c r="S36" s="96"/>
-      <c r="T36" s="97"/>
-      <c r="U36" s="96"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="81"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="84"/>
+      <c r="L36" s="83"/>
+      <c r="M36" s="85"/>
+      <c r="N36" s="85"/>
+      <c r="O36" s="96"/>
+      <c r="P36" s="87"/>
+      <c r="Q36" s="86"/>
+      <c r="R36" s="88"/>
+      <c r="S36" s="89"/>
+      <c r="T36" s="90"/>
+      <c r="U36" s="89"/>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="82"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="84"/>
-      <c r="D37" s="85"/>
-      <c r="E37" s="83"/>
+      <c r="A37" s="75"/>
+      <c r="B37" s="76"/>
+      <c r="C37" s="77"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="76"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="86"/>
-      <c r="H37" s="87"/>
-      <c r="I37" s="88"/>
-      <c r="J37" s="89"/>
-      <c r="K37" s="91"/>
-      <c r="L37" s="90"/>
-      <c r="M37" s="92"/>
-      <c r="N37" s="92"/>
-      <c r="O37" s="103"/>
-      <c r="P37" s="94"/>
-      <c r="Q37" s="93"/>
-      <c r="R37" s="95"/>
-      <c r="S37" s="96"/>
-      <c r="T37" s="97"/>
-      <c r="U37" s="96"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G37" s="79"/>
+      <c r="H37" s="80"/>
+      <c r="I37" s="81"/>
+      <c r="J37" s="82"/>
+      <c r="K37" s="84"/>
+      <c r="L37" s="83"/>
+      <c r="M37" s="85"/>
+      <c r="N37" s="85"/>
+      <c r="O37" s="96"/>
+      <c r="P37" s="87"/>
+      <c r="Q37" s="86"/>
+      <c r="R37" s="88"/>
+      <c r="S37" s="89"/>
+      <c r="T37" s="90"/>
+      <c r="U37" s="89"/>
+    </row>
+    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="75"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="76"/>
       <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>254</v>
-      </c>
-      <c r="C39" t="s">
-        <v>120</v>
-      </c>
-      <c r="D39" t="s">
-        <v>255</v>
-      </c>
-      <c r="E39" t="s">
-        <v>256</v>
-      </c>
+      <c r="G38" s="79"/>
+      <c r="H38" s="80"/>
+      <c r="I38" s="81"/>
+      <c r="J38" s="82"/>
+      <c r="K38" s="84"/>
+      <c r="L38" s="83"/>
+      <c r="M38" s="85"/>
+      <c r="N38" s="85"/>
+      <c r="O38" s="96"/>
+      <c r="P38" s="87"/>
+      <c r="Q38" s="86"/>
+      <c r="R38" s="88"/>
+      <c r="S38" s="89"/>
+      <c r="T38" s="90"/>
+      <c r="U38" s="89"/>
+    </row>
+    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="75"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="76"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="98" t="s">
-        <v>257</v>
-      </c>
+      <c r="G39" s="79"/>
+      <c r="H39" s="80"/>
+      <c r="I39" s="81"/>
+      <c r="J39" s="82"/>
+      <c r="K39" s="84"/>
+      <c r="L39" s="83"/>
+      <c r="M39" s="85"/>
+      <c r="N39" s="85"/>
+      <c r="O39" s="96"/>
+      <c r="P39" s="87"/>
+      <c r="Q39" s="86"/>
+      <c r="R39" s="88"/>
+      <c r="S39" s="89"/>
+      <c r="T39" s="90"/>
+      <c r="U39" s="89"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>258</v>
-      </c>
-      <c r="C40" t="s">
-        <v>127</v>
-      </c>
-      <c r="D40" t="s">
-        <v>154</v>
-      </c>
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="C41" t="s">
-        <v>260</v>
+        <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="E41" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="F41" s="4"/>
-      <c r="G41" s="98" t="s">
-        <v>128</v>
-      </c>
-      <c r="J41" t="s">
-        <v>140</v>
-      </c>
-      <c r="K41" t="s">
-        <v>246</v>
+      <c r="G41" s="91" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>263</v>
+        <v>249</v>
+      </c>
+      <c r="C42" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" t="s">
+        <v>130</v>
       </c>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>264</v>
+        <v>250</v>
+      </c>
+      <c r="C43" t="s">
+        <v>251</v>
+      </c>
+      <c r="D43" t="s">
+        <v>252</v>
+      </c>
+      <c r="E43" t="s">
+        <v>253</v>
       </c>
       <c r="F43" s="4"/>
+      <c r="G43" s="91" t="s">
+        <v>127</v>
+      </c>
+      <c r="J43" t="s">
+        <v>139</v>
+      </c>
+      <c r="K43" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>186</v>
-      </c>
-      <c r="E45" t="s">
-        <v>126</v>
+        <v>255</v>
       </c>
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>266</v>
-      </c>
-      <c r="E46" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>267</v>
+        <v>183</v>
       </c>
       <c r="E47" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="E48" t="s">
-        <v>170</v>
+        <v>243</v>
       </c>
       <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>129</v>
+        <v>258</v>
       </c>
       <c r="E49" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>269</v>
+        <v>259</v>
+      </c>
+      <c r="E50" t="s">
+        <v>167</v>
       </c>
       <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>270</v>
+        <v>128</v>
+      </c>
+      <c r="E51" t="s">
+        <v>138</v>
       </c>
       <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="F53" s="4"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>208</v>
+        <v>263</v>
       </c>
       <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>229</v>
+      </c>
       <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>273</v>
+        <v>205</v>
       </c>
       <c r="F57" s="4"/>
     </row>
@@ -4160,6 +4258,9 @@
       <c r="F58" s="4"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>264</v>
+      </c>
       <c r="F59" s="4"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -4201,480 +4302,484 @@
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F72" s="4"/>
     </row>
-    <row r="74" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F73" s="4"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F74" s="4"/>
+    </row>
     <row r="76" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>86</v>
-      </c>
-      <c r="C78" t="s">
-        <v>87</v>
-      </c>
-      <c r="E78" t="s">
-        <v>88</v>
-      </c>
-      <c r="J78" t="s">
-        <v>89</v>
-      </c>
-      <c r="L78" t="s">
-        <v>90</v>
-      </c>
-    </row>
+    <row r="78" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="80" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>94</v>
-      </c>
-    </row>
+        <v>86</v>
+      </c>
+      <c r="C80" t="s">
+        <v>87</v>
+      </c>
+      <c r="E80" t="s">
+        <v>88</v>
+      </c>
+      <c r="J80" t="s">
+        <v>89</v>
+      </c>
+      <c r="L80" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>274</v>
+        <v>84</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>275</v>
+        <v>85</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>319</v>
+      </c>
+    </row>
     <row r="172" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="173" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="174" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4790,17 +4895,13 @@
     <row r="284" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="285" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="286" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:U2">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4815,27 +4916,32 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L37">
-      <formula1>$C$41:$L$41</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L39">
+      <formula1>$C$43:$L$43</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K37">
-      <formula1>$C$40:$D$40</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K39">
+      <formula1>$C$42:$D$42</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A37">
-      <formula1>$C$39:$F$39</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A39">
+      <formula1>$C$41:$F$41</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3 M7 M5 M22:M23 M25:M37 N20 M11 M16 N17 N13">
-      <formula1>$A$43:$A$55</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3 M7 M5 M24:M25 M27:M39 N22 M11 M16 N17 N13">
+      <formula1>$A$45:$A$57</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3 N7 N5 N11 N16 N22:N23 N25:N37">
-      <formula1>$A$80:$A$169</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3 N7 N5 N11 N16 N24:N25 N27:N39">
+      <formula1>$A$82:$A$171</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
MA0703, MA0802 y MA0803: Escaletas y esqueletos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
@@ -1,29 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado08\guion02\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19203" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="246">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1171,6 +1167,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1214,18 +1222,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1288,7 +1284,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1323,7 +1319,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1534,127 +1530,128 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.265625" style="48" customWidth="1"/>
-    <col min="2" max="2" width="8.86328125" style="48" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.265625" style="48" customWidth="1"/>
-    <col min="5" max="5" width="27.1328125" style="48" customWidth="1"/>
-    <col min="6" max="6" width="5.265625" style="49" customWidth="1"/>
-    <col min="7" max="7" width="33.86328125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="4.06640625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="4.06640625" style="48" customWidth="1"/>
-    <col min="10" max="10" width="44.06640625" style="48" customWidth="1"/>
-    <col min="11" max="11" width="3.1328125" style="48" customWidth="1"/>
-    <col min="12" max="12" width="8.46484375" style="48" customWidth="1"/>
-    <col min="13" max="14" width="4.6640625" style="48" customWidth="1"/>
-    <col min="15" max="15" width="27.265625" style="50" customWidth="1"/>
-    <col min="16" max="16" width="2.1328125" style="48" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="48" customWidth="1"/>
-    <col min="18" max="18" width="4.265625" style="48" customWidth="1"/>
-    <col min="19" max="19" width="10.33203125" style="48" customWidth="1"/>
-    <col min="20" max="20" width="14.9296875" style="48" customWidth="1"/>
-    <col min="21" max="21" width="14.53125" style="48" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.6640625" style="48"/>
+    <col min="1" max="1" width="12.28515625" style="48" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="48" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" style="48" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" style="48" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" style="49" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="4" style="14" customWidth="1"/>
+    <col min="9" max="9" width="4" style="48" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" style="48" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="48" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" style="48" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="48" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="48" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" style="50" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" style="48" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" style="48" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="48" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" style="48" customWidth="1"/>
+    <col min="20" max="20" width="15" style="48" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" style="48" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.7109375" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="60" t="s">
+      <c r="J1" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="55" t="s">
+      <c r="N1" s="66"/>
+      <c r="O1" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="69" t="s">
+      <c r="R1" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="67" t="s">
+      <c r="S1" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="68" t="s">
+      <c r="T1" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="67" t="s">
+      <c r="U1" s="52" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="57"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="58"/>
+    <row r="2" spans="1:21" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="61"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="62"/>
       <c r="M2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="55"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="67"/>
-    </row>
-    <row r="3" spans="1:21" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="O2" s="59"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="52"/>
+    </row>
+    <row r="3" spans="1:21" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>96</v>
       </c>
@@ -1715,7 +1712,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>96</v>
       </c>
@@ -1776,7 +1773,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>96</v>
       </c>
@@ -1837,7 +1834,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>96</v>
       </c>
@@ -1898,7 +1895,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>96</v>
       </c>
@@ -1959,7 +1956,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>96</v>
       </c>
@@ -2020,7 +2017,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>96</v>
       </c>
@@ -2079,7 +2076,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>96</v>
       </c>
@@ -2092,7 +2089,9 @@
       <c r="D10" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="19"/>
+      <c r="E10" s="37" t="s">
+        <v>140</v>
+      </c>
       <c r="F10" s="30"/>
       <c r="G10" s="31" t="s">
         <v>221</v>
@@ -2136,7 +2135,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>96</v>
       </c>
@@ -2197,7 +2196,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>96</v>
       </c>
@@ -2258,7 +2257,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>96</v>
       </c>
@@ -2319,7 +2318,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>96</v>
       </c>
@@ -2380,7 +2379,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>96</v>
       </c>
@@ -2441,7 +2440,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>96</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>96</v>
       </c>
@@ -2563,7 +2562,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>96</v>
       </c>
@@ -2624,7 +2623,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>96</v>
       </c>
@@ -2637,7 +2636,9 @@
       <c r="D19" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E19" s="37"/>
+      <c r="E19" s="37" t="s">
+        <v>171</v>
+      </c>
       <c r="F19" s="30"/>
       <c r="G19" s="21" t="s">
         <v>174</v>
@@ -2675,7 +2676,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>96</v>
       </c>
@@ -2688,7 +2689,9 @@
       <c r="D20" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E20" s="37"/>
+      <c r="E20" s="37" t="s">
+        <v>171</v>
+      </c>
       <c r="F20" s="30"/>
       <c r="G20" s="21" t="s">
         <v>228</v>
@@ -2730,7 +2733,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>96</v>
       </c>
@@ -2743,7 +2746,9 @@
       <c r="D21" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E21" s="37"/>
+      <c r="E21" s="37" t="s">
+        <v>171</v>
+      </c>
       <c r="F21" s="30"/>
       <c r="G21" s="21" t="s">
         <v>216</v>
@@ -2783,13 +2788,13 @@
         <v>114</v>
       </c>
       <c r="T21" s="29" t="s">
-        <v>192</v>
+        <v>219</v>
       </c>
       <c r="U21" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>96</v>
       </c>
@@ -2848,7 +2853,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>96</v>
       </c>
@@ -2909,7 +2914,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>96</v>
       </c>
@@ -2970,7 +2975,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>96</v>
       </c>
@@ -3031,7 +3036,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>96</v>
       </c>
@@ -3092,7 +3097,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>96</v>
       </c>
@@ -3151,7 +3156,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>96</v>
       </c>
@@ -3210,7 +3215,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>96</v>
       </c>
@@ -3269,7 +3274,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>96</v>
       </c>
@@ -3314,7 +3319,7 @@
       <c r="T30" s="13"/>
       <c r="U30" s="12"/>
     </row>
-    <row r="31" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>96</v>
       </c>
@@ -3375,7 +3380,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>96</v>
       </c>
@@ -3433,12 +3438,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -3453,6 +3452,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L32">
@@ -3484,27 +3489,27 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.86328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" style="1"/>
-    <col min="14" max="14" width="24.265625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="69.86328125" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.3984375" style="1"/>
+    <col min="13" max="13" width="11.42578125" style="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="69.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3521,7 +3526,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -3545,7 +3550,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -3564,7 +3569,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -3583,7 +3588,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -3599,7 +3604,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -3616,7 +3621,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3633,7 +3638,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -3648,7 +3653,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -3663,7 +3668,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3678,7 +3683,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -3693,7 +3698,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -3708,7 +3713,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -3723,7 +3728,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -3738,7 +3743,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -3753,7 +3758,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -3768,7 +3773,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
@@ -3782,7 +3787,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1" t="s">
@@ -3796,7 +3801,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1" t="s">
@@ -3810,7 +3815,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
@@ -3824,7 +3829,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -3839,7 +3844,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -3854,7 +3859,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -3869,7 +3874,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -3884,7 +3889,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -3899,7 +3904,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -3914,7 +3919,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -3929,7 +3934,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -3944,7 +3949,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -3959,7 +3964,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -3974,7 +3979,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -3989,7 +3994,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -4004,7 +4009,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -4019,7 +4024,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -4034,7 +4039,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -4049,7 +4054,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -4064,7 +4069,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -4079,7 +4084,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -4094,7 +4099,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -4109,7 +4114,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -4124,7 +4129,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -4139,7 +4144,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -4154,7 +4159,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -4169,7 +4174,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -4184,7 +4189,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -4199,7 +4204,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -4214,7 +4219,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -4229,7 +4234,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -4244,7 +4249,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -4256,7 +4261,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -4268,7 +4273,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -4281,7 +4286,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -4294,7 +4299,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -4307,7 +4312,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -4320,7 +4325,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -4333,7 +4338,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -4346,7 +4351,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -4359,7 +4364,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -4372,7 +4377,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -4385,7 +4390,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -4398,7 +4403,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -4411,7 +4416,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -4424,7 +4429,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -4437,7 +4442,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -4450,7 +4455,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -4463,7 +4468,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -4476,7 +4481,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -4489,7 +4494,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -4502,7 +4507,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -4515,7 +4520,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -4528,7 +4533,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -4542,7 +4547,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -4556,7 +4561,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -4570,7 +4575,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -4584,7 +4589,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -4598,7 +4603,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -4612,7 +4617,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -4626,7 +4631,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -4640,7 +4645,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -4654,7 +4659,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -4668,7 +4673,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -4682,7 +4687,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -4696,7 +4701,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -4710,7 +4715,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -4724,7 +4729,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -4738,7 +4743,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -4752,7 +4757,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -4766,7 +4771,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -4780,7 +4785,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -4794,7 +4799,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -4808,7 +4813,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -4822,7 +4827,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -4836,7 +4841,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -4850,7 +4855,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -4864,7 +4869,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -4878,7 +4883,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -4892,7 +4897,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -4906,7 +4911,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -4920,7 +4925,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -4934,7 +4939,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -4948,7 +4953,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -4962,7 +4967,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -4976,7 +4981,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -4990,7 +4995,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -5004,7 +5009,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -5018,7 +5023,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -5032,7 +5037,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -5046,7 +5051,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -5060,7 +5065,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -5074,7 +5079,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -5088,7 +5093,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -5102,7 +5107,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -5116,7 +5121,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -5130,7 +5135,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -5144,7 +5149,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -5158,7 +5163,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -5172,7 +5177,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -5186,7 +5191,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -5200,7 +5205,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -5214,7 +5219,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -5228,7 +5233,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -5242,7 +5247,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -5256,7 +5261,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -5270,7 +5275,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -5284,7 +5289,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -5298,7 +5303,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -5312,7 +5317,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -5326,7 +5331,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -5340,7 +5345,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -5354,7 +5359,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -5368,7 +5373,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -5382,7 +5387,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -5396,7 +5401,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -5435,4 +5440,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización de escaleta mat 8 tema 2
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -577,9 +577,6 @@
     <t>Interactivo que permite estudiar la división sintética y el teorema del residuo</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: El teorema del resto</t>
-  </si>
-  <si>
     <t>Practica el teorema del resto</t>
   </si>
   <si>
@@ -794,6 +791,9 @@
   </si>
   <si>
     <t>Andrea</t>
+  </si>
+  <si>
+    <t>El teorema del resto</t>
   </si>
 </sst>
 </file>
@@ -1282,6 +1282,18 @@
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1325,18 +1337,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1645,9 +1645,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T29" sqref="T29"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q22" sqref="Q22:U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1676,94 +1676,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="E1" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="79" t="s">
+      <c r="J1" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="78" t="s">
+      <c r="K1" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="77" t="s">
+      <c r="L1" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="80" t="s">
+      <c r="M1" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="81"/>
-      <c r="O1" s="74" t="s">
+      <c r="N1" s="85"/>
+      <c r="O1" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="85" t="s">
+      <c r="P1" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="Q1" s="85" t="s">
+      <c r="Q1" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="88" t="s">
+      <c r="R1" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="86" t="s">
+      <c r="S1" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="87" t="s">
+      <c r="T1" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="86" t="s">
+      <c r="U1" s="71" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="76"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="77"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="81"/>
       <c r="M2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="74"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="86"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="86"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="71"/>
     </row>
     <row r="3" spans="1:22" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
@@ -1773,7 +1773,7 @@
         <v>97</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D3" s="55" t="s">
         <v>98</v>
@@ -1783,7 +1783,7 @@
       </c>
       <c r="F3" s="56"/>
       <c r="G3" s="54" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H3" s="57">
         <v>1</v>
@@ -1823,10 +1823,10 @@
         <v>107</v>
       </c>
       <c r="U3" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="V3" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1837,7 +1837,7 @@
         <v>97</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D4" s="49" t="s">
         <v>98</v>
@@ -1887,7 +1887,7 @@
         <v>115</v>
       </c>
       <c r="U4" s="49" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1898,7 +1898,7 @@
         <v>97</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>98</v>
@@ -1945,13 +1945,13 @@
         <v>114</v>
       </c>
       <c r="T5" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U5" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="V5" s="27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1962,7 +1962,7 @@
         <v>97</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D6" s="49" t="s">
         <v>98</v>
@@ -2023,7 +2023,7 @@
         <v>97</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>98</v>
@@ -2070,10 +2070,10 @@
         <v>114</v>
       </c>
       <c r="T7" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U7" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="35" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2084,7 +2084,7 @@
         <v>97</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>98</v>
@@ -2134,7 +2134,7 @@
         <v>133</v>
       </c>
       <c r="U8" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2145,7 +2145,7 @@
         <v>97</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D9" s="37" t="s">
         <v>98</v>
@@ -2175,7 +2175,7 @@
       <c r="M9" s="37"/>
       <c r="N9" s="37"/>
       <c r="O9" s="37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P9" s="37" t="s">
         <v>99</v>
@@ -2204,7 +2204,7 @@
         <v>97</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D10" s="37" t="s">
         <v>98</v>
@@ -2212,7 +2212,7 @@
       <c r="E10" s="40"/>
       <c r="F10" s="38"/>
       <c r="G10" s="39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H10" s="37">
         <v>8</v>
@@ -2221,7 +2221,7 @@
         <v>99</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K10" s="37" t="s">
         <v>99</v>
@@ -2232,7 +2232,7 @@
       <c r="M10" s="37"/>
       <c r="N10" s="37"/>
       <c r="O10" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P10" s="37" t="s">
         <v>99</v>
@@ -2247,7 +2247,7 @@
         <v>137</v>
       </c>
       <c r="T10" s="42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U10" s="42" t="s">
         <v>139</v>
@@ -2262,7 +2262,7 @@
         <v>97</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D11" s="37" t="s">
         <v>98</v>
@@ -2294,7 +2294,7 @@
         <v>69</v>
       </c>
       <c r="O11" s="37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P11" s="37" t="s">
         <v>99</v>
@@ -2309,10 +2309,10 @@
         <v>114</v>
       </c>
       <c r="T11" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="U11" s="37" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:22" s="35" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2323,7 +2323,7 @@
         <v>97</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>143</v>
@@ -2373,7 +2373,7 @@
         <v>148</v>
       </c>
       <c r="U12" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2384,7 +2384,7 @@
         <v>97</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D13" s="57" t="s">
         <v>143</v>
@@ -2437,7 +2437,7 @@
         <v>156</v>
       </c>
       <c r="V13" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="41" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2448,7 +2448,7 @@
         <v>97</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D14" s="37" t="s">
         <v>143</v>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="F14" s="38"/>
       <c r="G14" s="39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H14" s="37">
         <v>12</v>
@@ -2498,7 +2498,7 @@
         <v>159</v>
       </c>
       <c r="U14" s="37" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2509,7 +2509,7 @@
         <v>97</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>160</v>
@@ -2559,10 +2559,10 @@
         <v>165</v>
       </c>
       <c r="U15" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="V15" s="27" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2573,7 +2573,7 @@
         <v>97</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D16" s="49" t="s">
         <v>160</v>
@@ -2623,7 +2623,7 @@
         <v>170</v>
       </c>
       <c r="U16" s="49" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2634,7 +2634,7 @@
         <v>97</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D17" s="57" t="s">
         <v>160</v>
@@ -2662,7 +2662,7 @@
         <v>101</v>
       </c>
       <c r="M17" s="57" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N17" s="57"/>
       <c r="O17" s="57" t="s">
@@ -2681,13 +2681,13 @@
         <v>106</v>
       </c>
       <c r="T17" s="57" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U17" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="V17" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2698,7 +2698,7 @@
         <v>97</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>160</v>
@@ -2708,7 +2708,7 @@
       </c>
       <c r="F18" s="22"/>
       <c r="G18" s="44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H18" s="14">
         <v>16</v>
@@ -2717,7 +2717,7 @@
         <v>104</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>99</v>
@@ -2745,13 +2745,13 @@
         <v>114</v>
       </c>
       <c r="T18" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U18" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="V18" s="59" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2762,7 +2762,7 @@
         <v>97</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D19" s="49" t="s">
         <v>160</v>
@@ -2813,7 +2813,7 @@
         <v>97</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D20" s="57" t="s">
         <v>160</v>
@@ -2821,7 +2821,7 @@
       <c r="E20" s="57"/>
       <c r="F20" s="60"/>
       <c r="G20" s="54" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H20" s="57">
         <v>18</v>
@@ -2830,16 +2830,16 @@
         <v>104</v>
       </c>
       <c r="J20" s="57" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K20" s="57"/>
       <c r="L20" s="57"/>
       <c r="M20" s="57" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N20" s="57"/>
       <c r="O20" s="57" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P20" s="57" t="s">
         <v>99</v>
@@ -2851,16 +2851,16 @@
         <v>113</v>
       </c>
       <c r="S20" s="67" t="s">
+        <v>232</v>
+      </c>
+      <c r="T20" s="68" t="s">
         <v>233</v>
       </c>
-      <c r="T20" s="68" t="s">
-        <v>234</v>
-      </c>
       <c r="U20" s="67" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="V20" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W20" s="69"/>
     </row>
@@ -2872,7 +2872,7 @@
         <v>97</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>160</v>
@@ -2880,7 +2880,7 @@
       <c r="E21" s="14"/>
       <c r="F21" s="22"/>
       <c r="G21" s="44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H21" s="14">
         <v>19</v>
@@ -2889,7 +2889,7 @@
         <v>104</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K21" s="14" t="s">
         <v>104</v>
@@ -2902,7 +2902,7 @@
         <v>83</v>
       </c>
       <c r="O21" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P21" s="14" t="s">
         <v>99</v>
@@ -2917,13 +2917,13 @@
         <v>114</v>
       </c>
       <c r="T21" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U21" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="V21" s="27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2934,7 +2934,7 @@
         <v>97</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D22" s="49" t="s">
         <v>160</v>
@@ -2964,24 +2964,24 @@
       <c r="M22" s="64"/>
       <c r="N22" s="49"/>
       <c r="O22" s="49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P22" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="Q22" s="49" t="s">
+      <c r="Q22" t="s">
         <v>123</v>
       </c>
-      <c r="R22" s="49" t="s">
+      <c r="R22" t="s">
         <v>124</v>
       </c>
-      <c r="S22" s="49" t="s">
+      <c r="S22" t="s">
         <v>125</v>
       </c>
-      <c r="T22" s="49" t="s">
-        <v>179</v>
-      </c>
-      <c r="U22" s="49" t="s">
+      <c r="T22" t="s">
+        <v>251</v>
+      </c>
+      <c r="U22" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2993,7 +2993,7 @@
         <v>97</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D23" s="49" t="s">
         <v>160</v>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H23" s="49">
         <v>21</v>
@@ -3012,7 +3012,7 @@
         <v>104</v>
       </c>
       <c r="J23" s="49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K23" s="49" t="s">
         <v>104</v>
@@ -3025,7 +3025,7 @@
         <v>80</v>
       </c>
       <c r="O23" s="49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P23" s="49" t="s">
         <v>99</v>
@@ -3040,7 +3040,7 @@
         <v>125</v>
       </c>
       <c r="T23" s="49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U23" s="49" t="s">
         <v>126</v>
@@ -3055,7 +3055,7 @@
         <v>97</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D24" s="49" t="s">
         <v>160</v>
@@ -3065,7 +3065,7 @@
       </c>
       <c r="F24" s="51"/>
       <c r="G24" s="52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H24" s="49">
         <v>22</v>
@@ -3074,7 +3074,7 @@
         <v>104</v>
       </c>
       <c r="J24" s="49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K24" s="49" t="s">
         <v>104</v>
@@ -3087,7 +3087,7 @@
         <v>69</v>
       </c>
       <c r="O24" s="49" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P24" s="49" t="s">
         <v>99</v>
@@ -3102,10 +3102,10 @@
         <v>114</v>
       </c>
       <c r="T24" s="49" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="U24" s="49" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3116,17 +3116,17 @@
         <v>97</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E25" s="49" t="s">
         <v>140</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="52" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H25" s="49">
         <v>23</v>
@@ -3135,7 +3135,7 @@
         <v>104</v>
       </c>
       <c r="J25" s="49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K25" s="49" t="s">
         <v>104</v>
@@ -3148,7 +3148,7 @@
         <v>81</v>
       </c>
       <c r="O25" s="49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P25" s="49" t="s">
         <v>104</v>
@@ -3163,10 +3163,10 @@
         <v>114</v>
       </c>
       <c r="T25" s="49" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U25" s="49" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3177,17 +3177,17 @@
         <v>97</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>140</v>
       </c>
       <c r="F26" s="22"/>
       <c r="G26" s="46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H26" s="14">
         <v>24</v>
@@ -3196,7 +3196,7 @@
         <v>104</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K26" s="14" t="s">
         <v>104</v>
@@ -3209,7 +3209,7 @@
         <v>83</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P26" s="14" t="s">
         <v>104</v>
@@ -3224,13 +3224,13 @@
         <v>114</v>
       </c>
       <c r="T26" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U26" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="V26" s="59" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="W26" s="45"/>
     </row>
@@ -3242,15 +3242,15 @@
         <v>97</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="60"/>
       <c r="G27" s="57" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H27" s="57">
         <v>25</v>
@@ -3259,7 +3259,7 @@
         <v>104</v>
       </c>
       <c r="J27" s="57" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K27" s="57" t="s">
         <v>104</v>
@@ -3268,11 +3268,11 @@
         <v>101</v>
       </c>
       <c r="M27" s="55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N27" s="58"/>
       <c r="O27" s="57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P27" s="57" t="s">
         <v>99</v>
@@ -3287,13 +3287,13 @@
         <v>106</v>
       </c>
       <c r="T27" s="57" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="U27" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="V27" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3304,10 +3304,10 @@
         <v>97</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D28" s="49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E28" s="49"/>
       <c r="F28" s="51"/>
@@ -3321,7 +3321,7 @@
         <v>104</v>
       </c>
       <c r="J28" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K28" s="66" t="s">
         <v>99</v>
@@ -3334,7 +3334,7 @@
         <v>82</v>
       </c>
       <c r="O28" s="49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P28" s="49" t="s">
         <v>99</v>
@@ -3363,15 +3363,15 @@
         <v>97</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D29" s="49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E29" s="49"/>
       <c r="F29" s="51"/>
       <c r="G29" s="49" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H29" s="65">
         <v>27</v>
@@ -3380,7 +3380,7 @@
         <v>104</v>
       </c>
       <c r="J29" s="49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K29" s="50" t="s">
         <v>104</v>
@@ -3393,7 +3393,7 @@
         <v>80</v>
       </c>
       <c r="O29" s="49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P29" s="49" t="s">
         <v>99</v>
@@ -3408,10 +3408,10 @@
         <v>114</v>
       </c>
       <c r="T29" s="49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U29" s="49" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3422,10 +3422,10 @@
         <v>97</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E30" s="24" t="s">
         <v>10</v>
@@ -3439,18 +3439,18 @@
       </c>
       <c r="I30" s="19"/>
       <c r="J30" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K30" s="25" t="s">
         <v>104</v>
       </c>
       <c r="L30" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M30" s="21"/>
       <c r="N30" s="21"/>
       <c r="O30" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P30" s="8"/>
       <c r="Q30" s="9"/>
@@ -3467,17 +3467,17 @@
         <v>97</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H31" s="14">
         <v>29</v>
@@ -3486,7 +3486,7 @@
         <v>104</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K31" s="43" t="s">
         <v>104</v>
@@ -3499,7 +3499,7 @@
         <v>83</v>
       </c>
       <c r="O31" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P31" s="14" t="s">
         <v>99</v>
@@ -3514,13 +3514,13 @@
         <v>106</v>
       </c>
       <c r="T31" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U31" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="V31" s="27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3531,15 +3531,15 @@
         <v>97</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E32" s="24"/>
       <c r="F32" s="22"/>
       <c r="G32" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H32" s="4">
         <v>30</v>
@@ -3570,10 +3570,10 @@
         <v>114</v>
       </c>
       <c r="T32" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="U32" s="11" t="s">
         <v>236</v>
-      </c>
-      <c r="U32" s="11" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="33" spans="15:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3611,12 +3611,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -3631,6 +3625,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L32">

</xml_diff>

<commit_message>
Indicación en color de recursos en greco para Oliver
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
@@ -880,7 +880,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1031,6 +1031,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -1135,7 +1141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1338,6 +1344,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1645,9 +1655,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q22" sqref="Q22:U22"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2969,19 +2979,19 @@
       <c r="P22" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="Q22" s="89" t="s">
         <v>123</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22" s="89" t="s">
         <v>124</v>
       </c>
-      <c r="S22" t="s">
+      <c r="S22" s="89" t="s">
         <v>125</v>
       </c>
-      <c r="T22" t="s">
+      <c r="T22" s="89" t="s">
         <v>251</v>
       </c>
-      <c r="U22" t="s">
+      <c r="U22" s="89" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3339,19 +3349,19 @@
       <c r="P28" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="Q28" s="49" t="s">
+      <c r="Q28" s="90" t="s">
         <v>153</v>
       </c>
-      <c r="R28" s="49" t="s">
+      <c r="R28" s="90" t="s">
         <v>124</v>
       </c>
-      <c r="S28" s="49" t="s">
+      <c r="S28" s="90" t="s">
         <v>154</v>
       </c>
-      <c r="T28" s="49" t="s">
+      <c r="T28" s="90" t="s">
         <v>155</v>
       </c>
-      <c r="U28" s="49" t="s">
+      <c r="U28" s="90" t="s">
         <v>156</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización escaleta y cuaderno de estudio
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion02\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -18,12 +13,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="252">
   <si>
     <t>Asignatura</t>
   </si>
@@ -724,9 +719,6 @@
     <t xml:space="preserve">Competencias: El proceso de la construcción del álgebra </t>
   </si>
   <si>
-    <t>Competencias: Las expresiones algebraicas</t>
-  </si>
-  <si>
     <t>Interactivo para comprender qué es el lenguaje algebraico</t>
   </si>
   <si>
@@ -791,6 +783,12 @@
   </si>
   <si>
     <t>Problemas que implican operaciones con expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Evaluación: Expresiones y operaciones algebraicas</t>
+  </si>
+  <si>
+    <t>Las expresiones algebraicas</t>
   </si>
 </sst>
 </file>
@@ -1122,9 +1120,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1175,6 +1170,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1271,7 +1269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1306,7 +1304,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1517,9 +1515,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1534,10 +1532,11 @@
     <col min="8" max="8" width="4" style="5" customWidth="1"/>
     <col min="9" max="9" width="4" style="9" customWidth="1"/>
     <col min="10" max="10" width="44" style="9" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" style="9" customWidth="1"/>
-    <col min="13" max="14" width="4.7109375" style="9" customWidth="1"/>
-    <col min="15" max="15" width="27.28515625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="9" style="9" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" style="9" customWidth="1"/>
+    <col min="15" max="15" width="3" style="11" customWidth="1"/>
     <col min="16" max="16" width="9.5703125" style="9" customWidth="1"/>
     <col min="17" max="17" width="5.7109375" style="9" customWidth="1"/>
     <col min="18" max="18" width="4.28515625" style="9" customWidth="1"/>
@@ -1623,10 +1622,10 @@
       <c r="J2" s="51"/>
       <c r="K2" s="51"/>
       <c r="L2" s="51"/>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="N2" s="26" t="s">
         <v>77</v>
       </c>
       <c r="O2" s="48"/>
@@ -1638,66 +1637,66 @@
       <c r="U2" s="48"/>
     </row>
     <row r="3" spans="1:22" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="H3" s="32">
+      <c r="H3" s="31">
         <v>1</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="I3" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="J3" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="K3" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="32" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="P3" s="32" t="s">
+      <c r="P3" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q3" s="32">
+      <c r="Q3" s="31">
         <v>6</v>
       </c>
-      <c r="R3" s="32" t="s">
+      <c r="R3" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="S3" s="32" t="s">
+      <c r="S3" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="T3" s="32" t="s">
+      <c r="T3" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="U3" s="32" t="s">
+      <c r="U3" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="V3" s="24"/>
+      <c r="V3" s="23"/>
     </row>
     <row r="4" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
@@ -1712,51 +1711,51 @@
       <c r="D4" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="31" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="31">
         <v>2</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J4" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="K4" s="32" t="s">
+      <c r="J4" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="K4" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L4" s="32" t="s">
+      <c r="L4" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M4" s="35"/>
-      <c r="N4" s="32" t="s">
+      <c r="M4" s="34"/>
+      <c r="N4" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="32" t="s">
+      <c r="O4" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="P4" s="32" t="s">
+      <c r="P4" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q4" s="32">
+      <c r="Q4" s="31">
         <v>6</v>
       </c>
-      <c r="R4" s="32" t="s">
+      <c r="R4" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="S4" s="32" t="s">
+      <c r="S4" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="T4" s="32" t="s">
+      <c r="T4" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="U4" s="32" t="s">
+      <c r="U4" s="31" t="s">
         <v>210</v>
       </c>
     </row>
@@ -1773,51 +1772,51 @@
       <c r="D5" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="31" t="s">
+      <c r="F5" s="33"/>
+      <c r="G5" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="31">
         <v>3</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J5" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="K5" s="32" t="s">
+      <c r="J5" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="K5" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M5" s="32"/>
-      <c r="N5" s="29" t="s">
+      <c r="M5" s="31"/>
+      <c r="N5" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="O5" s="32" t="s">
+      <c r="O5" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="P5" s="32" t="s">
+      <c r="P5" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q5" s="32">
+      <c r="Q5" s="31">
         <v>6</v>
       </c>
-      <c r="R5" s="32" t="s">
+      <c r="R5" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="S5" s="32" t="s">
+      <c r="S5" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="T5" s="32" t="s">
+      <c r="T5" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="U5" s="32" t="s">
+      <c r="U5" s="31" t="s">
         <v>210</v>
       </c>
     </row>
@@ -1834,173 +1833,173 @@
       <c r="D6" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="34"/>
-      <c r="G6" s="31" t="s">
+      <c r="F6" s="33"/>
+      <c r="G6" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="31">
         <v>4</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="K6" s="32" t="s">
+      <c r="K6" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="L6" s="32" t="s">
+      <c r="L6" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32" t="s">
+      <c r="M6" s="31"/>
+      <c r="N6" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="O6" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="P6" s="32" t="s">
+      <c r="P6" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="Q6" s="32" t="s">
+      <c r="Q6" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="R6" s="32" t="s">
+      <c r="R6" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="S6" s="32" t="s">
+      <c r="S6" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="T6" s="32" t="s">
+      <c r="T6" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="U6" s="32" t="s">
+      <c r="U6" s="31" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="31" t="s">
+      <c r="F7" s="33"/>
+      <c r="G7" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="31">
         <v>5</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="M7" s="31"/>
+      <c r="N7" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="P7" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q7" s="31">
+        <v>6</v>
+      </c>
+      <c r="R7" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="S7" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="T7" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="U7" s="31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="33"/>
+      <c r="G8" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" s="31">
+        <v>6</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="K7" s="32" t="s">
+      <c r="K8" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L7" s="32" t="s">
+      <c r="L8" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M7" s="32"/>
-      <c r="N7" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="O7" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="P7" s="32" t="s">
+      <c r="M8" s="31"/>
+      <c r="N8" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="O8" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="P8" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q7" s="32">
+      <c r="Q8" s="31">
         <v>6</v>
       </c>
-      <c r="R7" s="32" t="s">
+      <c r="R8" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="S7" s="32" t="s">
+      <c r="S8" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="T7" s="32" t="s">
-        <v>215</v>
-      </c>
-      <c r="U7" s="32" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" s="34"/>
-      <c r="G8" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="H8" s="32">
-        <v>6</v>
-      </c>
-      <c r="I8" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="J8" s="32" t="s">
-        <v>239</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="L8" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="O8" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="P8" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q8" s="32">
-        <v>6</v>
-      </c>
-      <c r="R8" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="S8" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="T8" s="32" t="s">
+      <c r="T8" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="U8" s="32" t="s">
+      <c r="U8" s="31" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2017,128 +2016,128 @@
       <c r="D9" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="31" t="s">
+      <c r="F9" s="33"/>
+      <c r="G9" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="31">
         <v>7</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L9" s="32" t="s">
+      <c r="L9" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32" t="s">
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="P9" s="32" t="s">
+      <c r="P9" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q9" s="36" t="s">
+      <c r="Q9" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="R9" s="36" t="s">
+      <c r="R9" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="S9" s="36" t="s">
+      <c r="S9" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="T9" s="36" t="s">
+      <c r="T9" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="U9" s="36" t="s">
+      <c r="U9" s="35" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="31" t="s">
+      <c r="E10" s="28"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="31">
         <v>8</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="J10" s="32" t="s">
-        <v>240</v>
-      </c>
-      <c r="K10" s="32" t="s">
+      <c r="J10" s="31" t="s">
+        <v>239</v>
+      </c>
+      <c r="K10" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="L10" s="32" t="s">
+      <c r="L10" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32" t="s">
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="P10" s="32" t="s">
+      <c r="P10" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q10" s="36" t="s">
+      <c r="Q10" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="R10" s="36" t="s">
+      <c r="R10" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="S10" s="36" t="s">
+      <c r="S10" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="T10" s="36" t="s">
+      <c r="T10" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="U10" s="36" t="s">
+      <c r="U10" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="V10" s="44"/>
+      <c r="V10" s="43"/>
     </row>
     <row r="11" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="31" t="s">
         <v>135</v>
       </c>
       <c r="F11" s="18"/>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="45" t="s">
         <v>136</v>
       </c>
       <c r="H11" s="16">
@@ -2148,7 +2147,7 @@
         <v>103</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>103</v>
@@ -2183,146 +2182,146 @@
       </c>
     </row>
     <row r="12" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="31" t="s">
+      <c r="F12" s="33"/>
+      <c r="G12" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="31">
         <v>10</v>
       </c>
-      <c r="I12" s="32" t="s">
+      <c r="I12" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J12" s="32" t="s">
+      <c r="J12" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="K12" s="32" t="s">
+      <c r="K12" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L12" s="32" t="s">
+      <c r="L12" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32" t="s">
+      <c r="M12" s="31"/>
+      <c r="N12" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="O12" s="32" t="s">
+      <c r="O12" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="P12" s="32" t="s">
+      <c r="P12" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q12" s="32">
+      <c r="Q12" s="31">
         <v>6</v>
       </c>
-      <c r="R12" s="32" t="s">
+      <c r="R12" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="S12" s="32" t="s">
+      <c r="S12" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="T12" s="32" t="s">
+      <c r="T12" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="U12" s="32" t="s">
+      <c r="U12" s="31" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="31" t="s">
+      <c r="F13" s="33"/>
+      <c r="G13" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="31">
         <v>11</v>
       </c>
-      <c r="I13" s="32" t="s">
+      <c r="I13" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="K13" s="32" t="s">
+      <c r="K13" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="L13" s="32" t="s">
+      <c r="L13" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="M13" s="32" t="s">
+      <c r="M13" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32" t="s">
+      <c r="N13" s="31"/>
+      <c r="O13" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="P13" s="32" t="s">
+      <c r="P13" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="Q13" s="32" t="s">
+      <c r="Q13" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="R13" s="32" t="s">
+      <c r="R13" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="S13" s="32" t="s">
+      <c r="S13" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="T13" s="32" t="s">
+      <c r="T13" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="U13" s="32" t="s">
+      <c r="U13" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="V13" s="24"/>
+      <c r="V13" s="23"/>
     </row>
     <row r="14" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="31" t="s">
         <v>135</v>
       </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="45" t="s">
         <v>192</v>
       </c>
       <c r="H14" s="16">
@@ -2332,7 +2331,7 @@
         <v>103</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>103</v>
@@ -2379,51 +2378,51 @@
       <c r="D15" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="31" t="s">
+      <c r="F15" s="33"/>
+      <c r="G15" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="31">
         <v>13</v>
       </c>
-      <c r="I15" s="32" t="s">
+      <c r="I15" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="32" t="s">
-        <v>241</v>
-      </c>
-      <c r="K15" s="32" t="s">
+      <c r="J15" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="K15" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L15" s="32" t="s">
+      <c r="L15" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32" t="s">
+      <c r="M15" s="31"/>
+      <c r="N15" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="O15" s="32" t="s">
+      <c r="O15" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="P15" s="32" t="s">
+      <c r="P15" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q15" s="32">
+      <c r="Q15" s="31">
         <v>6</v>
       </c>
-      <c r="R15" s="32" t="s">
+      <c r="R15" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="S15" s="32" t="s">
+      <c r="S15" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="T15" s="32" t="s">
+      <c r="T15" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="U15" s="32" t="s">
+      <c r="U15" s="31" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2440,115 +2439,115 @@
       <c r="D16" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="31" t="s">
+      <c r="F16" s="33"/>
+      <c r="G16" s="45" t="s">
         <v>221</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="31">
         <v>14</v>
       </c>
-      <c r="I16" s="32" t="s">
+      <c r="I16" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J16" s="32" t="s">
+      <c r="J16" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="K16" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="L16" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="M16" s="31"/>
+      <c r="N16" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="O16" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="P16" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q16" s="31">
+        <v>6</v>
+      </c>
+      <c r="R16" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="S16" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="T16" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="U16" s="31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="F17" s="33"/>
+      <c r="G17" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="K16" s="32" t="s">
+      <c r="H17" s="31">
+        <v>15</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>243</v>
+      </c>
+      <c r="K17" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L16" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="M16" s="32"/>
-      <c r="N16" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="O16" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="P16" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q16" s="32">
+      <c r="L17" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="M17" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="P17" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q17" s="31">
         <v>6</v>
       </c>
-      <c r="R16" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="S16" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="T16" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="U16" s="32" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="F17" s="34"/>
-      <c r="G17" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="H17" s="32">
-        <v>15</v>
-      </c>
-      <c r="I17" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="J17" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="K17" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="L17" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="M17" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="P17" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q17" s="32">
-        <v>6</v>
-      </c>
-      <c r="R17" s="32" t="s">
+      <c r="R17" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="S17" s="32" t="s">
+      <c r="S17" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="T17" s="32" t="s">
+      <c r="T17" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="U17" s="32" t="s">
+      <c r="U17" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="V17" s="24"/>
+      <c r="V17" s="23"/>
     </row>
     <row r="18" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
@@ -2563,54 +2562,54 @@
       <c r="D18" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="31" t="s">
+      <c r="F18" s="33"/>
+      <c r="G18" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="31">
         <v>16</v>
       </c>
-      <c r="I18" s="32" t="s">
+      <c r="I18" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="K18" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="L18" s="32" t="s">
+      <c r="L18" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32" t="s">
+      <c r="M18" s="31"/>
+      <c r="N18" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="O18" s="32" t="s">
+      <c r="O18" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="P18" s="37" t="s">
+      <c r="P18" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="Q18" s="32">
+      <c r="Q18" s="31">
         <v>6</v>
       </c>
-      <c r="R18" s="32" t="s">
+      <c r="R18" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="S18" s="32" t="s">
+      <c r="S18" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="T18" s="32" t="s">
+      <c r="T18" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="U18" s="32" t="s">
+      <c r="U18" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="V18" s="24"/>
+      <c r="V18" s="23"/>
     </row>
     <row r="19" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
@@ -2625,216 +2624,218 @@
       <c r="D19" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="31" t="s">
+      <c r="F19" s="33"/>
+      <c r="G19" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="31">
         <v>17</v>
       </c>
-      <c r="I19" s="32" t="s">
+      <c r="I19" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J19" s="32" t="s">
+      <c r="J19" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32" t="s">
+      <c r="K19" s="31"/>
+      <c r="L19" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32" t="s">
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q19" s="32" t="s">
+      <c r="Q19" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="R19" s="32" t="s">
+      <c r="R19" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="S19" s="32" t="s">
+      <c r="S19" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="T19" s="32" t="s">
+      <c r="T19" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="U19" s="32" t="s">
+      <c r="U19" s="31" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E20" s="32" t="s">
+      <c r="E20" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="F20" s="34"/>
-      <c r="G20" s="31" t="s">
+      <c r="F20" s="33"/>
+      <c r="G20" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="H20" s="31">
+        <v>18</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="J20" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="K20" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="L20" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="O20" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="P20" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q20" s="31">
+        <v>6</v>
+      </c>
+      <c r="R20" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="S20" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="T20" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="U20" s="31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="33"/>
+      <c r="G21" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="H20" s="32">
-        <v>18</v>
-      </c>
-      <c r="I20" s="32" t="s">
+      <c r="H21" s="31">
+        <v>19</v>
+      </c>
+      <c r="I21" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J20" s="32" t="s">
-        <v>234</v>
-      </c>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32" t="s">
+      <c r="J21" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="M20" s="32" t="s">
+      <c r="M21" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32" t="s">
+      <c r="N21" s="31"/>
+      <c r="O21" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="P20" s="32" t="s">
+      <c r="P21" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q20" s="35">
+      <c r="Q21" s="34">
         <v>6</v>
       </c>
-      <c r="R20" s="35" t="s">
+      <c r="R21" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="S20" s="35" t="s">
+      <c r="S21" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="T20" s="38" t="s">
+      <c r="T21" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="U20" s="35" t="s">
+      <c r="U21" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="V20" s="24"/>
-      <c r="W20" s="26"/>
-    </row>
-    <row r="21" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="V21" s="23"/>
+      <c r="W21" s="25"/>
+    </row>
+    <row r="22" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C22" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D22" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E22" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="19" t="s">
+      <c r="F22" s="33"/>
+      <c r="G22" s="30" t="s">
         <v>222</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16" t="s">
+      <c r="H22" s="16">
+        <v>20</v>
+      </c>
+      <c r="I22" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="J21" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="K21" s="32" t="s">
+      <c r="J22" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="K22" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L21" s="32" t="s">
+      <c r="L22" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="32" t="s">
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="45"/>
-      <c r="U21" s="20"/>
-      <c r="V21" s="28"/>
-      <c r="W21" s="26"/>
-    </row>
-    <row r="22" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="H22" s="32">
-        <v>19</v>
-      </c>
-      <c r="I22" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="J22" s="32" t="s">
-        <v>246</v>
-      </c>
-      <c r="K22" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="L22" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="O22" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="P22" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q22" s="32">
-        <v>6</v>
-      </c>
-      <c r="R22" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="S22" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="T22" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="U22" s="32" t="s">
-        <v>210</v>
-      </c>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="44"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="25"/>
     </row>
     <row r="23" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -2849,49 +2850,49 @@
       <c r="D23" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="F23" s="34"/>
-      <c r="G23" s="31" t="s">
+      <c r="F23" s="33"/>
+      <c r="G23" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="H23" s="32">
-        <v>20</v>
-      </c>
-      <c r="I23" s="32" t="s">
+      <c r="H23" s="31">
+        <v>21</v>
+      </c>
+      <c r="I23" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="J23" s="32" t="s">
+      <c r="J23" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="K23" s="39" t="s">
+      <c r="K23" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="L23" s="32" t="s">
+      <c r="L23" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="M23" s="40"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="32" t="s">
+      <c r="M23" s="39"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="P23" s="32" t="s">
+      <c r="P23" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q23" s="41" t="s">
+      <c r="Q23" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="R23" s="41" t="s">
+      <c r="R23" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="S23" s="41" t="s">
+      <c r="S23" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="T23" s="41" t="s">
+      <c r="T23" s="40" t="s">
         <v>218</v>
       </c>
-      <c r="U23" s="41" t="s">
+      <c r="U23" s="40" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2908,54 +2909,54 @@
       <c r="D24" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="31" t="s">
+      <c r="F24" s="33"/>
+      <c r="G24" s="45" t="s">
         <v>224</v>
       </c>
-      <c r="H24" s="32">
-        <v>21</v>
-      </c>
-      <c r="I24" s="32" t="s">
+      <c r="H24" s="31">
+        <v>22</v>
+      </c>
+      <c r="I24" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J24" s="32" t="s">
-        <v>247</v>
-      </c>
-      <c r="K24" s="32" t="s">
+      <c r="J24" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="K24" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L24" s="32" t="s">
+      <c r="L24" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32" t="s">
+      <c r="M24" s="31"/>
+      <c r="N24" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="O24" s="32" t="s">
+      <c r="O24" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="P24" s="32" t="s">
+      <c r="P24" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q24" s="32" t="s">
+      <c r="Q24" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="R24" s="32" t="s">
+      <c r="R24" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="S24" s="32" t="s">
+      <c r="S24" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="T24" s="32" t="s">
+      <c r="T24" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="U24" s="32" t="s">
+      <c r="U24" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="V24" s="24"/>
+      <c r="V24" s="23"/>
     </row>
     <row r="25" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
@@ -2970,21 +2971,21 @@
       <c r="D25" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="19" t="s">
+      <c r="F25" s="33"/>
+      <c r="G25" s="45" t="s">
         <v>225</v>
       </c>
       <c r="H25" s="16">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I25" s="16" t="s">
         <v>103</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K25" s="16" t="s">
         <v>103</v>
@@ -3031,51 +3032,51 @@
       <c r="D26" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="E26" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="31" t="s">
+      <c r="F26" s="33"/>
+      <c r="G26" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="H26" s="32">
-        <v>23</v>
-      </c>
-      <c r="I26" s="32" t="s">
+      <c r="H26" s="31">
+        <v>24</v>
+      </c>
+      <c r="I26" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J26" s="32" t="s">
+      <c r="J26" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="K26" s="32" t="s">
+      <c r="K26" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L26" s="32" t="s">
+      <c r="L26" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M26" s="32"/>
-      <c r="N26" s="29" t="s">
+      <c r="M26" s="31"/>
+      <c r="N26" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="O26" s="32" t="s">
+      <c r="O26" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="P26" s="32" t="s">
+      <c r="P26" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="Q26" s="32">
+      <c r="Q26" s="31">
         <v>6</v>
       </c>
-      <c r="R26" s="32" t="s">
+      <c r="R26" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="S26" s="32" t="s">
+      <c r="S26" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="T26" s="32" t="s">
+      <c r="T26" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="U26" s="32" t="s">
+      <c r="U26" s="31" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3092,115 +3093,115 @@
       <c r="D27" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="31" t="s">
+      <c r="F27" s="33"/>
+      <c r="G27" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="H27" s="32">
-        <v>24</v>
-      </c>
-      <c r="I27" s="32" t="s">
+      <c r="H27" s="31">
+        <v>25</v>
+      </c>
+      <c r="I27" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J27" s="32" t="s">
+      <c r="J27" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="K27" s="32" t="s">
+      <c r="K27" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L27" s="32" t="s">
+      <c r="L27" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M27" s="32"/>
-      <c r="N27" s="32" t="s">
+      <c r="M27" s="31"/>
+      <c r="N27" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="O27" s="32" t="s">
+      <c r="O27" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="P27" s="32" t="s">
+      <c r="P27" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="Q27" s="32">
+      <c r="Q27" s="31">
         <v>6</v>
       </c>
-      <c r="R27" s="32" t="s">
+      <c r="R27" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="S27" s="32" t="s">
+      <c r="S27" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="T27" s="32" t="s">
+      <c r="T27" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="U27" s="32" t="s">
+      <c r="U27" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="V27" s="24"/>
-      <c r="W27" s="37"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="36"/>
     </row>
     <row r="28" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="E28" s="32"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="32" t="s">
+      <c r="E28" s="31"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="H28" s="32">
-        <v>25</v>
-      </c>
-      <c r="I28" s="32" t="s">
+      <c r="H28" s="31">
+        <v>26</v>
+      </c>
+      <c r="I28" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J28" s="32" t="s">
+      <c r="J28" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="K28" s="32" t="s">
+      <c r="K28" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L28" s="29" t="s">
+      <c r="L28" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="M28" s="29" t="s">
+      <c r="M28" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="N28" s="33"/>
-      <c r="O28" s="32" t="s">
+      <c r="N28" s="32"/>
+      <c r="O28" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="P28" s="32" t="s">
+      <c r="P28" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q28" s="32">
+      <c r="Q28" s="31">
         <v>6</v>
       </c>
-      <c r="R28" s="32" t="s">
+      <c r="R28" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="S28" s="32" t="s">
+      <c r="S28" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="T28" s="32" t="s">
+      <c r="T28" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="U28" s="32" t="s">
+      <c r="U28" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="V28" s="24"/>
+      <c r="V28" s="23"/>
     </row>
     <row r="29" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
@@ -3215,49 +3216,49 @@
       <c r="D29" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="E29" s="32"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="32" t="s">
+      <c r="E29" s="31"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="H29" s="42">
-        <v>26</v>
-      </c>
-      <c r="I29" s="32" t="s">
+      <c r="H29" s="41">
+        <v>27</v>
+      </c>
+      <c r="I29" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J29" s="32" t="s">
-        <v>248</v>
-      </c>
-      <c r="K29" s="33" t="s">
+      <c r="J29" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="K29" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="L29" s="29" t="s">
+      <c r="L29" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="M29" s="33"/>
-      <c r="N29" s="29" t="s">
+      <c r="M29" s="32"/>
+      <c r="N29" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="O29" s="32" t="s">
+      <c r="O29" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="P29" s="32" t="s">
+      <c r="P29" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="Q29" s="32" t="s">
+      <c r="Q29" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="R29" s="32" t="s">
+      <c r="R29" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="S29" s="32" t="s">
+      <c r="S29" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="T29" s="32" t="s">
+      <c r="T29" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="U29" s="32" t="s">
+      <c r="U29" s="31" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3274,49 +3275,49 @@
       <c r="D30" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="32" t="s">
-        <v>228</v>
-      </c>
-      <c r="H30" s="42">
-        <v>27</v>
-      </c>
-      <c r="I30" s="32" t="s">
+      <c r="E30" s="31"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="H30" s="41">
+        <v>28</v>
+      </c>
+      <c r="I30" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J30" s="32" t="s">
+      <c r="J30" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="K30" s="29" t="s">
+      <c r="K30" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="L30" s="29" t="s">
+      <c r="L30" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="M30" s="33"/>
-      <c r="N30" s="29" t="s">
+      <c r="M30" s="32"/>
+      <c r="N30" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="O30" s="32" t="s">
+      <c r="O30" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="P30" s="32" t="s">
+      <c r="P30" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="Q30" s="32">
+      <c r="Q30" s="31">
         <v>6</v>
       </c>
-      <c r="R30" s="32" t="s">
+      <c r="R30" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="S30" s="32" t="s">
+      <c r="S30" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="T30" s="32" t="s">
+      <c r="T30" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="U30" s="32" t="s">
+      <c r="U30" s="31" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3333,37 +3334,37 @@
       <c r="D31" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="34"/>
-      <c r="G31" s="32" t="s">
+      <c r="F31" s="33"/>
+      <c r="G31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="32">
-        <v>28</v>
-      </c>
-      <c r="I31" s="32"/>
-      <c r="J31" s="42" t="s">
-        <v>236</v>
-      </c>
-      <c r="K31" s="29" t="s">
+      <c r="H31" s="31">
+        <v>29</v>
+      </c>
+      <c r="I31" s="31"/>
+      <c r="J31" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="K31" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="L31" s="29" t="s">
+      <c r="L31" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="32" t="s">
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="31" t="s">
         <v>185</v>
       </c>
-      <c r="P31" s="42"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="42"/>
-      <c r="S31" s="42"/>
-      <c r="T31" s="42"/>
-      <c r="U31" s="42"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="41"/>
+      <c r="S31" s="41"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="41"/>
     </row>
     <row r="32" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
@@ -3378,51 +3379,51 @@
       <c r="D32" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="E32" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="F32" s="34"/>
-      <c r="G32" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="H32" s="32">
-        <v>29</v>
-      </c>
-      <c r="I32" s="32" t="s">
+      <c r="F32" s="33"/>
+      <c r="G32" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="H32" s="31">
+        <v>30</v>
+      </c>
+      <c r="I32" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J32" s="32" t="s">
-        <v>237</v>
-      </c>
-      <c r="K32" s="29" t="s">
+      <c r="J32" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="K32" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="L32" s="29" t="s">
+      <c r="L32" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29" t="s">
+      <c r="M32" s="28"/>
+      <c r="N32" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="O32" s="32" t="s">
+      <c r="O32" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="P32" s="32" t="s">
+      <c r="P32" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q32" s="32">
+      <c r="Q32" s="31">
         <v>6</v>
       </c>
-      <c r="R32" s="32" t="s">
+      <c r="R32" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="S32" s="32" t="s">
+      <c r="S32" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="T32" s="32" t="s">
+      <c r="T32" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="U32" s="32" t="s">
+      <c r="U32" s="31" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3439,77 +3440,77 @@
       <c r="D33" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="32" t="s">
+      <c r="E33" s="31"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="H33" s="32">
-        <v>30</v>
-      </c>
-      <c r="I33" s="32" t="s">
+      <c r="H33" s="31">
+        <v>31</v>
+      </c>
+      <c r="I33" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="J33" s="32" t="s">
-        <v>249</v>
-      </c>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29" t="s">
+      <c r="J33" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29" t="s">
+      <c r="M33" s="28"/>
+      <c r="N33" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="O33" s="32"/>
-      <c r="P33" s="32" t="s">
+      <c r="O33" s="31"/>
+      <c r="P33" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="Q33" s="42">
+      <c r="Q33" s="41">
         <v>6</v>
       </c>
-      <c r="R33" s="42" t="s">
+      <c r="R33" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="S33" s="42" t="s">
+      <c r="S33" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="T33" s="43" t="s">
+      <c r="T33" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="U33" s="42" t="s">
+      <c r="U33" s="41" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O34" s="25"/>
+      <c r="O34" s="24"/>
     </row>
     <row r="35" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O35" s="25"/>
+      <c r="O35" s="24"/>
     </row>
     <row r="36" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O36" s="25"/>
+      <c r="O36" s="24"/>
     </row>
     <row r="37" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O37" s="25"/>
+      <c r="O37" s="24"/>
     </row>
     <row r="38" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O38" s="25"/>
+      <c r="O38" s="24"/>
     </row>
     <row r="39" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O39" s="25"/>
+      <c r="O39" s="24"/>
     </row>
     <row r="40" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O40" s="25"/>
+      <c r="O40" s="24"/>
     </row>
     <row r="41" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O41" s="25"/>
+      <c r="O41" s="24"/>
     </row>
     <row r="42" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O42" s="25"/>
+      <c r="O42" s="24"/>
     </row>
     <row r="43" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O43" s="25"/>
+      <c r="O43" s="24"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:U2">
@@ -3538,7 +3539,7 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:N3 N13 N17 M16:N16 M11:N11 N23 M28:N33 M25:N26 M5:N5 M7:N7 K3:L33 A3:A33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:N3 N13 N17 M16:N16 M11:N11 N23 M28:N33 M25:N26 M5:N5 M7:N7 K3:L22 K23:L33 A3:A22 A23:A33">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Revisión tema 2 grado 8
Se realizan cambios en el orden de los recursos del tema 2 de grado 8,
se actualiza escaleta y cuaderno de estudio.
Se anexa archivo con observaciones.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/Escaleta_MA_08_02_CO.xlsx
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="251">
   <si>
     <t>Asignatura</t>
   </si>
@@ -320,9 +320,6 @@
     <t>MA_08_02_CO</t>
   </si>
   <si>
-    <t>Expresiones algebraicas</t>
-  </si>
-  <si>
     <t>Sí</t>
   </si>
   <si>
@@ -347,12 +344,6 @@
     <t>Recurso F8-01</t>
   </si>
   <si>
-    <t>Términos algebraicos</t>
-  </si>
-  <si>
-    <t>Conceptos claves de las expresiones algebraicas</t>
-  </si>
-  <si>
     <t xml:space="preserve">ACTIVIDAD </t>
   </si>
   <si>
@@ -368,15 +359,9 @@
     <t>Recurso M1B-01</t>
   </si>
   <si>
-    <t>El lenguaje algebraico</t>
-  </si>
-  <si>
     <t>Corresponde al REC20 del manuscrito original. Incluye una serie de enunciados en lenguaje natural, representados a partir de una imagen y se espera que el estudiante seleccione la respuesta correcta de la expresión en lenguaje algebraico que modele la situación.</t>
   </si>
   <si>
-    <t>Polinomios</t>
-  </si>
-  <si>
     <t>Repasa los conceptos básicos de los polinomios</t>
   </si>
   <si>
@@ -398,24 +383,15 @@
     <t>MT_10_02</t>
   </si>
   <si>
-    <t>Clasificación de las expresiones algebraicas</t>
-  </si>
-  <si>
     <t>Corresponde al REC40 del manuscrito original. El estudiante debe clasificar de ciertas expresiones cuáles son monomios, cuáles son polinomios y cuáles no son expresiones algebraicas.</t>
   </si>
   <si>
-    <t>Características de los polinomios</t>
-  </si>
-  <si>
     <t>Corresponde al REC50 del manuscrito original.  La idea es completar huecos dependiendo de ciertas frases que involucran los conceptos de polinomio completo, polinomio opuesto, entre otros.</t>
   </si>
   <si>
     <t>Recurso M2A-01</t>
   </si>
   <si>
-    <t>Valor numérico de un polinomio</t>
-  </si>
-  <si>
     <t>Actividad para ejercitar la evaluación numérica de los polinomios</t>
   </si>
   <si>
@@ -437,12 +413,6 @@
     <t>Refuerza tu aprendizaje: Las expresiones algebraicas</t>
   </si>
   <si>
-    <t>Operaciones aditivas entre polinomios</t>
-  </si>
-  <si>
-    <t>Adición y sustracción de expresiones algebraicas</t>
-  </si>
-  <si>
     <t>Actividad para practicar la adición y la sustracción de polinomios</t>
   </si>
   <si>
@@ -479,12 +449,6 @@
     <t>Recurso M101A-02</t>
   </si>
   <si>
-    <t>Operaciones multiplicativas entre polinomios</t>
-  </si>
-  <si>
-    <t>Propiedades de los exponentes</t>
-  </si>
-  <si>
     <t>Practica la ley de los exponentes</t>
   </si>
   <si>
@@ -494,16 +458,10 @@
     <t>Recurso M9B-01</t>
   </si>
   <si>
-    <t>Multiplicación de expresiones algebraicas</t>
-  </si>
-  <si>
     <t>Corresponde al REC120 del manuscrito original. Se presentan varios ejercicios en el que se debe multiplicar polinomios. El estudiante debe ubicar la respuesta frente a cada polinomio.</t>
   </si>
   <si>
     <t>Recurso M2A-02</t>
-  </si>
-  <si>
-    <t>División de expresiones algebraicas</t>
   </si>
   <si>
     <t>La construcción del interactivo se realizará de la siguiente manera: en la diapositiva 1, se incluirá el ejemplo de división entre expresiones algebraicas que propone el autor en la IMG06; en la diapositiva 2 se incluirán con un color distinto los ejemplos de división de monomios; en la diapositiva 3 se incluirá el ejemplo propuesto por el autor de división de un polinomio por un monomio, pero se sugiere indicar con un color distinto la dvisión de cada término del polinomio por el monomio y el resultado del respectivo color; en la diapositiva 4 se incluirá la explicación del algoritmo de división entre dos polinomios y se pueden aprovechar como ejemplo la IMG07 o la IMG08 propuestas por el autor en el manuscrito.</t>
@@ -544,9 +502,6 @@
     <t>Actividad para resolver problemas usando el teorema del residuo</t>
   </si>
   <si>
-    <t>Operaciones combinadas entre polinomios</t>
-  </si>
-  <si>
     <t>Actividad para ejercitar las operaciones combinadas entre polinomios</t>
   </si>
   <si>
@@ -556,9 +511,6 @@
     <t>Recurso M2C-02</t>
   </si>
   <si>
-    <t>Resolución de problemas aplicando expresiones algebraicas</t>
-  </si>
-  <si>
     <t>Actividad para resolver situaciones problema empleando expresiones algebraicas</t>
   </si>
   <si>
@@ -697,103 +649,148 @@
     <t>El teorema del resto</t>
   </si>
   <si>
-    <t>La adición y la sustracción de polinomios</t>
-  </si>
-  <si>
     <t>Las operaciones aditivas entre polinomios</t>
   </si>
   <si>
+    <t>La división de polinomios</t>
+  </si>
+  <si>
+    <t>Practica el teorema del residuo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competencias: El proceso de la construcción del álgebra </t>
+  </si>
+  <si>
+    <t>Interactivo para comprender qué es el lenguaje algebraico</t>
+  </si>
+  <si>
+    <t>Actividad para recordar los conceptos claves del álgebra</t>
+  </si>
+  <si>
+    <t>Actividad para interpretar expresiones cotidianas en lenguaje algebraico y viceversa</t>
+  </si>
+  <si>
+    <t>Actividad sobre Las expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Actividad sobre Las operaciones aditivas entre polinomios</t>
+  </si>
+  <si>
+    <t>Interactivo que explica como dividir dos polinomios</t>
+  </si>
+  <si>
+    <t>Actividad sobre La multiplicación y la división de polinomios</t>
+  </si>
+  <si>
+    <t>Mapa conceptual del tema Expresiones y operaciones algebraicas</t>
+  </si>
+  <si>
+    <t>Evalúa tus conocimientos sobre Expresiones y operaciones algebraicas</t>
+  </si>
+  <si>
+    <t>Actividad para diferenciar entre monomios, polinomios y expresiones no polinómicas</t>
+  </si>
+  <si>
+    <t>Actividad para recordar y ejercitar las carácterísticas de los polinomios</t>
+  </si>
+  <si>
+    <t>Interactivo para repasar conceptos relativos al álgebra</t>
+  </si>
+  <si>
+    <t>Actividad para practicar la ley de los exponentes</t>
+  </si>
+  <si>
+    <t>Actividad para practicar la multiplicación de polinomios</t>
+  </si>
+  <si>
+    <t>La división de expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Interactivo para estudiar y practicar la división de expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Actividad sobre La división de polinomios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para resolver situaciones problema  </t>
+  </si>
+  <si>
+    <t>Actividad para resolver problemas utilizando el teorema del residuo</t>
+  </si>
+  <si>
+    <t>Actividad para ejercitar las operaciones básicas con los polinomios</t>
+  </si>
+  <si>
+    <t>Motor que incluye actividades de respuesta abierta del tema Expresiones y operaciones algebraicas</t>
+  </si>
+  <si>
+    <t>Las expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Relaciona conceptos de las expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Traduce expresiones al lenguaje algebraico</t>
+  </si>
+  <si>
+    <t>Clasifica expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Calcula el valor numérico de un polinomio</t>
+  </si>
+  <si>
+    <t>Resuelve adiciones y sustracciones de polinomios</t>
+  </si>
+  <si>
+    <t>Practica la multiplicación de polinomios</t>
+  </si>
+  <si>
+    <t>Resuelve problemas que implican expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las operaciones multiplicativas entre polinomios</t>
+  </si>
+  <si>
+    <t>Practica las operaciones combinadas entre polinomios</t>
+  </si>
+  <si>
+    <t>Soluciona problemas aplicando expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Comunica lo aprendido de las expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Ejercita la división de polinomios</t>
+  </si>
+  <si>
+    <t>Las variables, las incognitas y las constantes</t>
+  </si>
+  <si>
+    <t>Reconoce las características de los polinomios</t>
+  </si>
+  <si>
+    <t>El valor numerico de un polinomio</t>
+  </si>
+  <si>
+    <t>La sustracción de polinomios</t>
+  </si>
+  <si>
+    <t>Las operaciones multiplicativas entre polinomios</t>
+  </si>
+  <si>
+    <t>Ley de los exponentes para la multiplicación, el cociente y la potenciación</t>
+  </si>
+  <si>
+    <t>La multiplicación de expresiones algebraicas</t>
+  </si>
+  <si>
+    <t>Polinomios opuestos</t>
+  </si>
+  <si>
     <t>La multiplicación de polinomios</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: La división de polinomios</t>
-  </si>
-  <si>
-    <t>La división de polinomios</t>
-  </si>
-  <si>
-    <t>Practica el teorema del residuo</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: La multiplicación y la división de polinomios</t>
-  </si>
-  <si>
-    <t>Las operaciones combinadas entre polinomios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Competencias: El proceso de la construcción del álgebra </t>
-  </si>
-  <si>
-    <t>Interactivo para comprender qué es el lenguaje algebraico</t>
-  </si>
-  <si>
-    <t>Actividad para recordar los conceptos claves del álgebra</t>
-  </si>
-  <si>
-    <t>Actividad para interpretar expresiones cotidianas en lenguaje algebraico y viceversa</t>
-  </si>
-  <si>
-    <t>Actividad sobre Las expresiones algebraicas</t>
-  </si>
-  <si>
-    <t>Actividad sobre Las operaciones aditivas entre polinomios</t>
-  </si>
-  <si>
-    <t>Interactivo que explica como dividir dos polinomios</t>
-  </si>
-  <si>
-    <t>Actividad sobre La multiplicación y la división de polinomios</t>
-  </si>
-  <si>
-    <t>Mapa conceptual del tema Expresiones y operaciones algebraicas</t>
-  </si>
-  <si>
-    <t>Evalúa tus conocimientos sobre Expresiones y operaciones algebraicas</t>
-  </si>
-  <si>
-    <t>Actividad para diferenciar entre monomios, polinomios y expresiones no polinómicas</t>
-  </si>
-  <si>
-    <t>Actividad para recordar y ejercitar las carácterísticas de los polinomios</t>
-  </si>
-  <si>
-    <t>Interactivo para repasar conceptos relativos al álgebra</t>
-  </si>
-  <si>
-    <t>Actividad para practicar la ley de los exponentes</t>
-  </si>
-  <si>
-    <t>Actividad para practicar la multiplicación de polinomios</t>
-  </si>
-  <si>
-    <t>La división de expresiones algebraicas</t>
-  </si>
-  <si>
-    <t>Interactivo para estudiar y practicar la división de expresiones algebraicas</t>
-  </si>
-  <si>
-    <t>Actividad sobre La división de polinomios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad para resolver situaciones problema  </t>
-  </si>
-  <si>
-    <t>Actividad para resolver problemas utilizando el teorema del residuo</t>
-  </si>
-  <si>
-    <t>Actividad para ejercitar las operaciones básicas con los polinomios</t>
-  </si>
-  <si>
-    <t>Motor que incluye actividades de respuesta abierta del tema Expresiones y operaciones algebraicas</t>
-  </si>
-  <si>
-    <t>Problemas que implican operaciones con expresiones algebraicas</t>
-  </si>
-  <si>
-    <t>Evaluación: Expresiones y operaciones algebraicas</t>
-  </si>
-  <si>
-    <t>Las expresiones algebraicas</t>
+    <t>La división entre dos polinomios</t>
   </si>
 </sst>
 </file>
@@ -880,7 +877,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -939,12 +936,6 @@
       <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1081,7 +1072,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1109,41 +1100,34 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1164,20 +1148,31 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1522,7 +1517,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1532,236 +1527,236 @@
     <col min="3" max="3" width="26.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" style="9" customWidth="1"/>
     <col min="5" max="5" width="27.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="10" customWidth="1"/>
     <col min="7" max="7" width="33.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="4" style="5" customWidth="1"/>
-    <col min="9" max="9" width="4" style="9" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12" style="9" customWidth="1"/>
     <col min="10" max="10" width="44" style="9" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="9" customWidth="1"/>
     <col min="12" max="12" width="9" style="9" customWidth="1"/>
-    <col min="13" max="13" width="3.42578125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" style="9" customWidth="1"/>
-    <col min="15" max="15" width="3" style="11" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" style="9" customWidth="1"/>
-    <col min="18" max="18" width="4.28515625" style="9" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" style="9" customWidth="1"/>
+    <col min="15" max="15" width="22.85546875" style="11" customWidth="1"/>
+    <col min="16" max="16" width="20" style="9" customWidth="1"/>
+    <col min="17" max="17" width="14" style="9" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" style="9" customWidth="1"/>
+    <col min="19" max="19" width="13" style="9" customWidth="1"/>
     <col min="20" max="20" width="15" style="9" customWidth="1"/>
     <col min="21" max="21" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="10.7109375" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="53"/>
-      <c r="O1" s="46" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="46" t="s">
+      <c r="S1" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="48" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="26" t="s">
+      <c r="A2" s="52"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
     </row>
     <row r="3" spans="1:22" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="D3" s="21" t="s">
+      <c r="C3" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="F3" s="26"/>
+      <c r="G3" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="J3" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3" s="42"/>
+      <c r="O3" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="H3" s="31">
-        <v>1</v>
-      </c>
-      <c r="I3" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="J3" s="31" t="s">
+      <c r="Q3" s="28">
+        <v>6</v>
+      </c>
+      <c r="R3" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="T3" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="U3" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="V3" s="20"/>
+    </row>
+    <row r="4" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="K3" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L3" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="N3" s="32"/>
-      <c r="O3" s="31" t="s">
+      <c r="E4" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="G4" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="H4" s="6">
+        <v>2</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="P3" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q3" s="31">
+      <c r="J4" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M4" s="43"/>
+      <c r="N4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q4" s="28">
         <v>6</v>
       </c>
-      <c r="R3" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="S3" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="T3" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="U3" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="V3" s="23"/>
-    </row>
-    <row r="4" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="45" t="s">
+      <c r="R4" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="31">
-        <v>2</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="K4" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L4" s="31" t="s">
+      <c r="S4" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="M4" s="34"/>
-      <c r="N4" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="O4" s="31" t="s">
+      <c r="T4" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="P4" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q4" s="31">
-        <v>6</v>
-      </c>
-      <c r="R4" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S4" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T4" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="U4" s="31" t="s">
-        <v>210</v>
+      <c r="U4" s="28" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1772,240 +1767,244 @@
         <v>97</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="D5" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="F5" s="30"/>
+      <c r="G5" s="39" t="s">
+        <v>230</v>
+      </c>
+      <c r="H5" s="6">
+        <v>3</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="45" t="s">
+      <c r="Q5" s="28">
+        <v>6</v>
+      </c>
+      <c r="R5" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S5" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="U5" s="28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="28">
+        <v>4</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="O6" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="31">
-        <v>3</v>
-      </c>
-      <c r="I5" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="K5" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L5" s="31" t="s">
+      <c r="P6" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q6" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="R6" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="U6" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="H7" s="6">
+        <v>5</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q7" s="28">
+        <v>6</v>
+      </c>
+      <c r="R7" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S7" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="M5" s="31"/>
-      <c r="N5" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="O5" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="P5" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q5" s="31">
+      <c r="T7" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="U7" s="28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>242</v>
+      </c>
+      <c r="H8" s="6">
         <v>6</v>
       </c>
-      <c r="R5" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S5" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T5" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="U5" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="I8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="P8" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="H6" s="31">
-        <v>4</v>
-      </c>
-      <c r="I6" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J6" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="K6" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="L6" s="31" t="s">
+      <c r="Q8" s="28">
+        <v>6</v>
+      </c>
+      <c r="R8" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S8" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="O6" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="P6" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q6" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="R6" s="31" t="s">
+      <c r="T8" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="S6" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="T6" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="U6" s="31" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="H7" s="31">
-        <v>5</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J7" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="K7" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L7" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M7" s="31"/>
-      <c r="N7" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="O7" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="P7" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q7" s="31">
-        <v>6</v>
-      </c>
-      <c r="R7" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S7" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T7" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="U7" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="H8" s="31">
-        <v>6</v>
-      </c>
-      <c r="I8" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>238</v>
-      </c>
-      <c r="K8" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L8" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="O8" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P8" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q8" s="31">
-        <v>6</v>
-      </c>
-      <c r="R8" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S8" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T8" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="U8" s="31" t="s">
-        <v>210</v>
+      <c r="U8" s="28" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2016,1315 +2015,1347 @@
         <v>97</v>
       </c>
       <c r="C9" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>243</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>232</v>
+      </c>
+      <c r="H9" s="6">
+        <v>7</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q9" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="R9" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="S9" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="T9" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U9" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>243</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="H10" s="6">
+        <v>8</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q10" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="R10" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="S10" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="T10" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="U10" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="V10" s="38"/>
+    </row>
+    <row r="11" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="6">
+        <v>9</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q11" s="15">
+        <v>6</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="S11" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="T11" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="U11" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="F12" s="30"/>
+      <c r="G12" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="H12" s="6">
+        <v>10</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q12" s="28">
+        <v>6</v>
+      </c>
+      <c r="R12" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S12" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="T12" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="U12" s="28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="F13" s="30"/>
+      <c r="G13" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="H13" s="28">
+        <v>11</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="M13" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="P13" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q13" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="R13" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="S13" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="T13" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="U13" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="V13" s="20"/>
+    </row>
+    <row r="14" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="H14" s="6">
+        <v>12</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>6</v>
+      </c>
+      <c r="R14" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="T14" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="U14" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="F15" s="30"/>
+      <c r="G15" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="H15" s="6">
+        <v>13</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q15" s="28">
+        <v>6</v>
+      </c>
+      <c r="R15" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S15" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="T15" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="U15" s="28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>234</v>
+      </c>
+      <c r="H16" s="6">
+        <v>14</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M16" s="6"/>
+      <c r="N16" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q16" s="28">
+        <v>6</v>
+      </c>
+      <c r="R16" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S16" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="T16" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="U16" s="28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F17" s="30"/>
+      <c r="G17" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="H17" s="28">
+        <v>15</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="K17" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="L17" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="M17" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="P17" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q17" s="28">
+        <v>6</v>
+      </c>
+      <c r="R17" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="S17" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="T17" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="U17" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="V17" s="20"/>
+    </row>
+    <row r="18" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="H18" s="6">
+        <v>16</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="P18" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q18" s="28">
+        <v>6</v>
+      </c>
+      <c r="R18" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S18" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="T18" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="U18" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="V18" s="20"/>
+    </row>
+    <row r="19" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="H19" s="6">
+        <v>17</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q19" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="R19" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="S19" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="T19" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="U19" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="H20" s="6">
+        <v>18</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q20" s="31">
+        <v>6</v>
+      </c>
+      <c r="R20" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S20" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="T20" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="U20" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="V20" s="20"/>
+      <c r="W20" s="22"/>
+    </row>
+    <row r="21" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F21" s="30"/>
+      <c r="G21" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="H21" s="28">
+        <v>19</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="K21" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="L21" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="34"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="22"/>
+    </row>
+    <row r="22" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F22" s="30"/>
+      <c r="G22" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="H22" s="28">
+        <v>20</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="K22" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="L22" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="O22" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="P22" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q22" s="28">
+        <v>6</v>
+      </c>
+      <c r="R22" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S22" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="T22" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="U22" s="28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="H23" s="6">
+        <v>21</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K23" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M23" s="46"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q23" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="R23" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="S23" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="T23" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="U23" s="35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G24" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="H24" s="6">
+        <v>22</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q24" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="R24" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="S24" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="T24" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="U24" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="V24" s="20"/>
+    </row>
+    <row r="25" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="H25" s="6">
+        <v>23</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M25" s="6"/>
+      <c r="N25" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q25" s="28">
+        <v>6</v>
+      </c>
+      <c r="R25" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S25" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="T25" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="U25" s="28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G26" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H26" s="6">
+        <v>24</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q26" s="28">
+        <v>6</v>
+      </c>
+      <c r="R26" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S26" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="T26" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="U26" s="28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F27" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" s="47">
+        <v>25</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="K27" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="L27" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="M27" s="42"/>
+      <c r="N27" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q27" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="R27" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="S27" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="T27" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="U27" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="V27" s="20"/>
+      <c r="W27" s="33"/>
+    </row>
+    <row r="28" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F28" s="30"/>
+      <c r="G28" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="H28" s="36">
+        <v>26</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="L28" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="M28" s="29"/>
+      <c r="N28" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="O28" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="P28" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q28" s="28">
+        <v>6</v>
+      </c>
+      <c r="R28" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S28" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="T28" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="U28" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="V28" s="20"/>
+      <c r="W28" s="40"/>
+    </row>
+    <row r="29" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" s="30"/>
+      <c r="G29" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="H29" s="6">
+        <v>27</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="K29" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M29" s="6"/>
+      <c r="N29" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="P29" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="H9" s="31">
-        <v>7</v>
-      </c>
-      <c r="I9" s="31" t="s">
+      <c r="Q29" s="15">
+        <v>6</v>
+      </c>
+      <c r="R29" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="S29" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="T29" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="U29" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="V29" s="20"/>
+      <c r="W29" s="40"/>
+    </row>
+    <row r="30" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E30" s="28"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="H30" s="6">
+        <v>26</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L30" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="M30" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="N30" s="42"/>
+      <c r="O30" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="P30" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q30" s="28">
+        <v>6</v>
+      </c>
+      <c r="R30" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="J9" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="K9" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L9" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31" t="s">
-        <v>188</v>
-      </c>
-      <c r="P9" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q9" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="R9" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="S9" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="T9" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="U9" s="35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="45" t="s">
-        <v>196</v>
-      </c>
-      <c r="H10" s="31">
-        <v>8</v>
-      </c>
-      <c r="I10" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="J10" s="31" t="s">
-        <v>239</v>
-      </c>
-      <c r="K10" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="L10" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31" t="s">
-        <v>195</v>
-      </c>
-      <c r="P10" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q10" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="R10" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="S10" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="T10" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="U10" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="V10" s="43"/>
-    </row>
-    <row r="11" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="H11" s="16">
-        <v>9</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="M11" s="16"/>
-      <c r="N11" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q11" s="16">
-        <v>6</v>
-      </c>
-      <c r="R11" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="S11" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="T11" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="U11" s="16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="45" t="s">
-        <v>219</v>
-      </c>
-      <c r="H12" s="31">
-        <v>10</v>
-      </c>
-      <c r="I12" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J12" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="K12" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L12" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="O12" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="P12" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q12" s="31">
-        <v>6</v>
-      </c>
-      <c r="R12" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S12" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T12" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="U12" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="H13" s="31">
-        <v>11</v>
-      </c>
-      <c r="I13" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="J13" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="K13" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="L13" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="M13" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="P13" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q13" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="R13" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="S13" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="T13" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="U13" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="V13" s="23"/>
-    </row>
-    <row r="14" spans="1:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="45" t="s">
-        <v>192</v>
-      </c>
-      <c r="H14" s="16">
-        <v>12</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="L14" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="O14" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="P14" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q14" s="16">
-        <v>6</v>
-      </c>
-      <c r="R14" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="S14" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="T14" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="U14" s="16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="H15" s="31">
-        <v>13</v>
-      </c>
-      <c r="I15" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J15" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="K15" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L15" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="O15" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="P15" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q15" s="31">
-        <v>6</v>
-      </c>
-      <c r="R15" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S15" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T15" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="U15" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="45" t="s">
-        <v>221</v>
-      </c>
-      <c r="H16" s="31">
-        <v>14</v>
-      </c>
-      <c r="I16" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J16" s="31" t="s">
-        <v>241</v>
-      </c>
-      <c r="K16" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L16" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M16" s="31"/>
-      <c r="N16" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="O16" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="P16" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q16" s="31">
-        <v>6</v>
-      </c>
-      <c r="R16" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S16" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T16" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="U16" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="30" t="s">
-        <v>242</v>
-      </c>
-      <c r="H17" s="31">
-        <v>15</v>
-      </c>
-      <c r="I17" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="J17" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="K17" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L17" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="M17" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="P17" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q17" s="31">
-        <v>6</v>
-      </c>
-      <c r="R17" s="31" t="s">
+      <c r="S30" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="S17" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="T17" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="U17" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="V17" s="23"/>
-    </row>
-    <row r="18" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="H18" s="31">
-        <v>16</v>
-      </c>
-      <c r="I18" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J18" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="K18" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="L18" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="O18" s="31" t="s">
+      <c r="T30" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="P18" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q18" s="31">
-        <v>6</v>
-      </c>
-      <c r="R18" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S18" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T18" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="U18" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="V18" s="23"/>
-    </row>
-    <row r="19" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="45" t="s">
-        <v>161</v>
-      </c>
-      <c r="H19" s="31">
-        <v>17</v>
-      </c>
-      <c r="I19" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J19" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q19" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="R19" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="S19" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="T19" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="U19" s="31" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="45" t="s">
-        <v>223</v>
-      </c>
-      <c r="H20" s="31">
-        <v>18</v>
-      </c>
-      <c r="I20" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J20" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="M20" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="P20" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q20" s="34">
-        <v>6</v>
-      </c>
-      <c r="R20" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="S20" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="T20" s="37" t="s">
-        <v>207</v>
-      </c>
-      <c r="U20" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="V20" s="23"/>
-      <c r="W20" s="25"/>
-    </row>
-    <row r="21" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="45" t="s">
-        <v>222</v>
-      </c>
-      <c r="H21" s="16">
-        <v>19</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="K21" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L21" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="44"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="25"/>
-    </row>
-    <row r="22" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="F22" s="33"/>
-      <c r="G22" s="45" t="s">
-        <v>249</v>
-      </c>
-      <c r="H22" s="31">
-        <v>20</v>
-      </c>
-      <c r="I22" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J22" s="31" t="s">
-        <v>245</v>
-      </c>
-      <c r="K22" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L22" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="O22" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="P22" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q22" s="31">
-        <v>6</v>
-      </c>
-      <c r="R22" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S22" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T22" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="U22" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="H23" s="31">
-        <v>21</v>
-      </c>
-      <c r="I23" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="J23" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="K23" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="L23" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="M23" s="39"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="P23" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q23" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="R23" s="40" t="s">
-        <v>121</v>
-      </c>
-      <c r="S23" s="40" t="s">
-        <v>122</v>
-      </c>
-      <c r="T23" s="40" t="s">
-        <v>218</v>
-      </c>
-      <c r="U23" s="40" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="45" t="s">
-        <v>224</v>
-      </c>
-      <c r="H24" s="31">
-        <v>22</v>
-      </c>
-      <c r="I24" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J24" s="31" t="s">
-        <v>246</v>
-      </c>
-      <c r="K24" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L24" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="O24" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="P24" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q24" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="R24" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="S24" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="T24" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="U24" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="V24" s="23"/>
-    </row>
-    <row r="25" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F25" s="33"/>
-      <c r="G25" s="45" t="s">
-        <v>225</v>
-      </c>
-      <c r="H25" s="16">
-        <v>23</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="K25" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="M25" s="16"/>
-      <c r="N25" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="O25" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="P25" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q25" s="16">
-        <v>6</v>
-      </c>
-      <c r="R25" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="S25" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="T25" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="U25" s="16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F26" s="33"/>
-      <c r="G26" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="H26" s="31">
-        <v>24</v>
-      </c>
-      <c r="I26" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J26" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="K26" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L26" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M26" s="31"/>
-      <c r="N26" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="O26" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="P26" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q26" s="31">
-        <v>6</v>
-      </c>
-      <c r="R26" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S26" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T26" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="U26" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="30" t="s">
-        <v>172</v>
-      </c>
-      <c r="H27" s="31">
-        <v>25</v>
-      </c>
-      <c r="I27" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J27" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="K27" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L27" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="O27" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="P27" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q27" s="31">
-        <v>6</v>
-      </c>
-      <c r="R27" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S27" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T27" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="U27" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="V27" s="23"/>
-      <c r="W27" s="36"/>
-    </row>
-    <row r="28" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="H28" s="31">
-        <v>26</v>
-      </c>
-      <c r="I28" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J28" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="K28" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L28" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="M28" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="N28" s="32"/>
-      <c r="O28" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="P28" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q28" s="31">
-        <v>6</v>
-      </c>
-      <c r="R28" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="S28" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="T28" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="U28" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="V28" s="23"/>
-    </row>
-    <row r="29" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="H29" s="41">
-        <v>27</v>
-      </c>
-      <c r="I29" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J29" s="31" t="s">
-        <v>247</v>
-      </c>
-      <c r="K29" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="L29" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="M29" s="32"/>
-      <c r="N29" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="O29" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="P29" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q29" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="R29" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="S29" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="T29" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="U29" s="31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="H30" s="41">
-        <v>28</v>
-      </c>
-      <c r="I30" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J30" s="31" t="s">
-        <v>181</v>
-      </c>
-      <c r="K30" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="L30" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="M30" s="32"/>
-      <c r="N30" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="O30" s="31" t="s">
-        <v>182</v>
-      </c>
-      <c r="P30" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q30" s="31">
-        <v>6</v>
-      </c>
-      <c r="R30" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="S30" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="T30" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="U30" s="31" t="s">
-        <v>210</v>
-      </c>
+      <c r="U30" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="V30" s="20"/>
     </row>
     <row r="31" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -3334,102 +3365,102 @@
         <v>97</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E31" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="E31" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="33"/>
-      <c r="G31" s="6" t="s">
+      <c r="F31" s="30"/>
+      <c r="G31" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="31">
+      <c r="H31" s="28">
         <v>29</v>
       </c>
-      <c r="I31" s="31"/>
-      <c r="J31" s="41" t="s">
-        <v>235</v>
-      </c>
-      <c r="K31" s="28" t="s">
+      <c r="I31" s="28"/>
+      <c r="J31" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="K31" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="L31" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="36"/>
+      <c r="U31" s="36"/>
+    </row>
+    <row r="32" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="F32" s="30"/>
+      <c r="G32" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H32" s="6">
+        <v>30</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="K32" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="L32" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q32" s="28">
+        <v>6</v>
+      </c>
+      <c r="R32" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="L31" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
-      <c r="O31" s="31" t="s">
-        <v>185</v>
-      </c>
-      <c r="P31" s="41"/>
-      <c r="Q31" s="41"/>
-      <c r="R31" s="41"/>
-      <c r="S31" s="41"/>
-      <c r="T31" s="41"/>
-      <c r="U31" s="41"/>
-    </row>
-    <row r="32" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="E32" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="H32" s="31">
-        <v>30</v>
-      </c>
-      <c r="I32" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J32" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="K32" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="L32" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="O32" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="P32" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q32" s="31">
-        <v>6</v>
-      </c>
-      <c r="R32" s="31" t="s">
+      <c r="S32" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="S32" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="T32" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="U32" s="31" t="s">
-        <v>210</v>
+      <c r="T32" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="U32" s="28" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3440,82 +3471,82 @@
         <v>97</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="H33" s="31">
+        <v>184</v>
+      </c>
+      <c r="E33" s="28"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="H33" s="28">
         <v>31</v>
       </c>
-      <c r="I33" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J33" s="31" t="s">
-        <v>248</v>
-      </c>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28" t="s">
+      <c r="I33" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J33" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="O33" s="28"/>
+      <c r="P33" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q33" s="36">
+        <v>6</v>
+      </c>
+      <c r="R33" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="S33" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="O33" s="31"/>
-      <c r="P33" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q33" s="41">
-        <v>6</v>
-      </c>
-      <c r="R33" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="S33" s="41" t="s">
-        <v>112</v>
-      </c>
-      <c r="T33" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="U33" s="41" t="s">
-        <v>210</v>
+      <c r="T33" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="U33" s="36" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O34" s="24"/>
+      <c r="O34" s="21"/>
     </row>
     <row r="35" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O35" s="24"/>
+      <c r="O35" s="21"/>
     </row>
     <row r="36" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O36" s="24"/>
+      <c r="O36" s="21"/>
     </row>
     <row r="37" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O37" s="24"/>
+      <c r="O37" s="21"/>
     </row>
     <row r="38" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O38" s="24"/>
+      <c r="O38" s="21"/>
     </row>
     <row r="39" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O39" s="24"/>
+      <c r="O39" s="21"/>
     </row>
     <row r="40" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O40" s="24"/>
+      <c r="O40" s="21"/>
     </row>
     <row r="41" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O41" s="24"/>
+      <c r="O41" s="21"/>
     </row>
     <row r="42" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O42" s="24"/>
+      <c r="O42" s="21"/>
     </row>
     <row r="43" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O43" s="24"/>
+      <c r="O43" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:U2">
@@ -3544,7 +3575,7 @@
     <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:N3 N13 N17 M16:N16 M11:N11 N23 M28:N33 M25:N26 M5:N5 M7:N7 K3:L19 K20:L33 A3:A19 A20:A33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:N3 N13 N17 M16:N16 M11:N11 N23 M5:N5 M7:N7 M25:N25 K3:L26 K27:N33 A3:A33">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>